<commit_message>
Work done on test cases
</commit_message>
<xml_diff>
--- a/TestCaseTemplateRBSUEljunia.xlsx
+++ b/TestCaseTemplateRBSUEljunia.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA Teamwork\BankAccountingSystem\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="255" windowWidth="19065" windowHeight="8205" activeTab="1"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
   <si>
     <t>Dependencies:</t>
   </si>
@@ -220,16 +225,113 @@
   </si>
   <si>
     <t>System prompts the user that password must be at least 6 characters; allows him to re-enter the attributes</t>
+  </si>
+  <si>
+    <t>Test article publish</t>
+  </si>
+  <si>
+    <t>Click the new article button</t>
+  </si>
+  <si>
+    <t>Write article headline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write article </t>
+  </si>
+  <si>
+    <t>Click post article button</t>
+  </si>
+  <si>
+    <t>Article options page is displayed</t>
+  </si>
+  <si>
+    <t>Article editing page is displayed</t>
+  </si>
+  <si>
+    <t>New article is published and displayed at main page</t>
+  </si>
+  <si>
+    <t>TC-4.5</t>
+  </si>
+  <si>
+    <t>Test article delete</t>
+  </si>
+  <si>
+    <t>Check if publish article functionality works</t>
+  </si>
+  <si>
+    <t>Check if article deletion functionality works</t>
+  </si>
+  <si>
+    <t>Click the delete article option</t>
+  </si>
+  <si>
+    <t>Article should not exist</t>
+  </si>
+  <si>
+    <t>Check if article exists</t>
+  </si>
+  <si>
+    <t>TC-4.6</t>
+  </si>
+  <si>
+    <t>TC-4.7</t>
+  </si>
+  <si>
+    <t>Test article editing</t>
+  </si>
+  <si>
+    <t>Check if article editing functionality works</t>
+  </si>
+  <si>
+    <t>Click the edit article option</t>
+  </si>
+  <si>
+    <t>Write new article headline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write new article </t>
+  </si>
+  <si>
+    <t>Article headline and content should be different</t>
+  </si>
+  <si>
+    <t>TC-4.8</t>
+  </si>
+  <si>
+    <t>Test User Account Viewing</t>
+  </si>
+  <si>
+    <t>Test if you can view any user accounts as an admin</t>
+  </si>
+  <si>
+    <t>Open users menu in admin panel</t>
+  </si>
+  <si>
+    <t>Find a user whos profile you whish to see</t>
+  </si>
+  <si>
+    <t>Click the account button on the right</t>
+  </si>
+  <si>
+    <t>Users page should be displaed</t>
+  </si>
+  <si>
+    <t>User page should be shown</t>
+  </si>
+  <si>
+    <t>Log in as admin and open article options</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;лв.&quot;_-;\-* #,##0.00\ &quot;лв.&quot;_-;_-* &quot;-&quot;??\ &quot;лв.&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -335,6 +437,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -676,14 +783,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -698,22 +807,20 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -722,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -852,27 +959,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -898,15 +984,9 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="6"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -921,12 +1001,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -945,18 +1019,81 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1003,7 +1140,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1035,9 +1172,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1069,6 +1207,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1244,14 +1383,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J349"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -1265,8 +1404,8 @@
     <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -1287,8 +1426,8 @@
       <c r="I1" s="20"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="51"/>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="75"/>
       <c r="B2" s="33" t="s">
         <v>16</v>
       </c>
@@ -1305,7 +1444,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="35"/>
       <c r="B3" s="36" t="s">
         <v>17</v>
@@ -1323,7 +1462,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="39"/>
       <c r="B4" s="36"/>
       <c r="C4" s="30"/>
@@ -1337,7 +1476,7 @@
       <c r="I4" s="20"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="25"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
@@ -1349,35 +1488,35 @@
       <c r="I5" s="20"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="49"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="73"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="71"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1391,7 +1530,7 @@
       <c r="I8" s="27"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="13.5" thickBot="1">
+    <row r="9" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="7"/>
       <c r="C9" s="6"/>
@@ -1403,7 +1542,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1">
+    <row r="10" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>18</v>
       </c>
@@ -1435,7 +1574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>24</v>
       </c>
@@ -1449,7 +1588,7 @@
       <c r="I11" s="9"/>
       <c r="J11" s="11"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
@@ -1461,7 +1600,7 @@
       <c r="I12" s="13"/>
       <c r="J12" s="15"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14"/>
@@ -1473,7 +1612,7 @@
       <c r="I13" s="13"/>
       <c r="J13" s="15"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
@@ -1485,7 +1624,7 @@
       <c r="I14" s="13"/>
       <c r="J14" s="15"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="14"/>
@@ -1497,7 +1636,7 @@
       <c r="I15" s="13"/>
       <c r="J15" s="15"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14"/>
@@ -1509,7 +1648,7 @@
       <c r="I16" s="13"/>
       <c r="J16" s="15"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="14"/>
@@ -1521,7 +1660,7 @@
       <c r="I17" s="13"/>
       <c r="J17" s="15"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
       <c r="C18" s="14"/>
@@ -1533,7 +1672,7 @@
       <c r="I18" s="13"/>
       <c r="J18" s="15"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="14"/>
@@ -1545,7 +1684,7 @@
       <c r="I19" s="13"/>
       <c r="J19" s="15"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
       <c r="C20" s="14"/>
@@ -1557,7 +1696,7 @@
       <c r="I20" s="13"/>
       <c r="J20" s="15"/>
     </row>
-    <row r="21" spans="1:10" ht="13.5" thickBot="1">
+    <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16"/>
       <c r="B21" s="17"/>
       <c r="C21" s="18"/>
@@ -1569,7 +1708,7 @@
       <c r="I21" s="17"/>
       <c r="J21" s="19"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="21"/>
       <c r="C22" s="20"/>
@@ -1581,7 +1720,7 @@
       <c r="I22" s="21"/>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="24"/>
       <c r="B23" s="21"/>
       <c r="C23" s="20"/>
@@ -1593,7 +1732,7 @@
       <c r="I23" s="21"/>
       <c r="J23" s="20"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="24"/>
       <c r="B24" s="21"/>
       <c r="C24" s="20"/>
@@ -1605,7 +1744,7 @@
       <c r="I24" s="21"/>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="21"/>
       <c r="C25" s="20"/>
@@ -1617,7 +1756,7 @@
       <c r="I25" s="21"/>
       <c r="J25" s="20"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="21"/>
       <c r="C26" s="20"/>
@@ -1629,7 +1768,7 @@
       <c r="I26" s="21"/>
       <c r="J26" s="20"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="21"/>
       <c r="C27" s="20"/>
@@ -1641,7 +1780,7 @@
       <c r="I27" s="21"/>
       <c r="J27" s="20"/>
     </row>
-    <row r="28" spans="1:10" ht="15" customHeight="1">
+    <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A28" s="20"/>
       <c r="B28" s="21"/>
       <c r="C28" s="28"/>
@@ -1653,7 +1792,7 @@
       <c r="I28" s="21"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="20"/>
       <c r="B29" s="21"/>
       <c r="C29" s="20"/>
@@ -1665,7 +1804,7 @@
       <c r="I29" s="21"/>
       <c r="J29" s="20"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
       <c r="B30" s="21"/>
       <c r="D30" s="20"/>
@@ -1676,7 +1815,7 @@
       <c r="I30" s="21"/>
       <c r="J30" s="20"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="20"/>
       <c r="B31" s="21"/>
       <c r="C31" s="20"/>
@@ -1688,7 +1827,7 @@
       <c r="I31" s="21"/>
       <c r="J31" s="20"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="20"/>
       <c r="B32" s="21"/>
       <c r="C32" s="20"/>
@@ -1700,7 +1839,7 @@
       <c r="I32" s="21"/>
       <c r="J32" s="20"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="20"/>
       <c r="B33" s="21"/>
       <c r="C33" s="20"/>
@@ -1712,7 +1851,7 @@
       <c r="I33" s="21"/>
       <c r="J33" s="20"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="20"/>
       <c r="B34" s="21"/>
       <c r="C34" s="20"/>
@@ -1724,7 +1863,7 @@
       <c r="I34" s="21"/>
       <c r="J34" s="20"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="20"/>
       <c r="B35" s="21"/>
       <c r="C35" s="20"/>
@@ -1736,7 +1875,7 @@
       <c r="I35" s="21"/>
       <c r="J35" s="20"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="20"/>
       <c r="B36" s="21"/>
       <c r="C36" s="20"/>
@@ -1748,7 +1887,7 @@
       <c r="I36" s="21"/>
       <c r="J36" s="20"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="20"/>
       <c r="B37" s="21"/>
       <c r="C37" s="20"/>
@@ -1760,7 +1899,7 @@
       <c r="I37" s="21"/>
       <c r="J37" s="20"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="20"/>
       <c r="B38" s="21"/>
       <c r="C38" s="20"/>
@@ -1772,7 +1911,7 @@
       <c r="I38" s="21"/>
       <c r="J38" s="20"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="20"/>
       <c r="B39" s="21"/>
       <c r="C39" s="20"/>
@@ -1784,7 +1923,7 @@
       <c r="I39" s="21"/>
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="20"/>
       <c r="B40" s="21"/>
       <c r="C40" s="20"/>
@@ -1796,7 +1935,7 @@
       <c r="I40" s="21"/>
       <c r="J40" s="20"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="20"/>
       <c r="B41" s="21"/>
       <c r="C41" s="20"/>
@@ -1808,7 +1947,7 @@
       <c r="I41" s="21"/>
       <c r="J41" s="20"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="20"/>
       <c r="B42" s="21"/>
       <c r="C42" s="20"/>
@@ -1820,7 +1959,7 @@
       <c r="I42" s="21"/>
       <c r="J42" s="20"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="20"/>
       <c r="B43" s="21"/>
       <c r="C43" s="20"/>
@@ -1832,7 +1971,7 @@
       <c r="I43" s="21"/>
       <c r="J43" s="20"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="20"/>
       <c r="B44" s="21"/>
       <c r="C44" s="20"/>
@@ -1844,7 +1983,7 @@
       <c r="I44" s="21"/>
       <c r="J44" s="20"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="20"/>
       <c r="B45" s="21"/>
       <c r="C45" s="20"/>
@@ -1856,7 +1995,7 @@
       <c r="I45" s="21"/>
       <c r="J45" s="20"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="20"/>
       <c r="B46" s="21"/>
       <c r="C46" s="20"/>
@@ -1868,7 +2007,7 @@
       <c r="I46" s="21"/>
       <c r="J46" s="20"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="20"/>
       <c r="B47" s="21"/>
       <c r="C47" s="20"/>
@@ -1880,7 +2019,7 @@
       <c r="I47" s="21"/>
       <c r="J47" s="20"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="20"/>
       <c r="B48" s="21"/>
       <c r="C48" s="20"/>
@@ -1892,7 +2031,7 @@
       <c r="I48" s="21"/>
       <c r="J48" s="20"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="20"/>
       <c r="B49" s="21"/>
       <c r="C49" s="20"/>
@@ -1904,7 +2043,7 @@
       <c r="I49" s="21"/>
       <c r="J49" s="20"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="20"/>
       <c r="B50" s="21"/>
       <c r="C50" s="20"/>
@@ -1916,7 +2055,7 @@
       <c r="I50" s="21"/>
       <c r="J50" s="20"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="20"/>
       <c r="B51" s="21"/>
       <c r="C51" s="20"/>
@@ -1928,7 +2067,7 @@
       <c r="I51" s="21"/>
       <c r="J51" s="20"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="20"/>
       <c r="B52" s="21"/>
       <c r="C52" s="20"/>
@@ -1940,7 +2079,7 @@
       <c r="I52" s="21"/>
       <c r="J52" s="20"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="20"/>
       <c r="B53" s="21"/>
       <c r="C53" s="20"/>
@@ -1952,7 +2091,7 @@
       <c r="I53" s="21"/>
       <c r="J53" s="20"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="20"/>
       <c r="B54" s="21"/>
       <c r="C54" s="20"/>
@@ -1964,7 +2103,7 @@
       <c r="I54" s="21"/>
       <c r="J54" s="20"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="20"/>
       <c r="B55" s="21"/>
       <c r="C55" s="20"/>
@@ -1976,7 +2115,7 @@
       <c r="I55" s="21"/>
       <c r="J55" s="20"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="20"/>
       <c r="B56" s="21"/>
       <c r="C56" s="20"/>
@@ -1988,7 +2127,7 @@
       <c r="I56" s="21"/>
       <c r="J56" s="20"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="20"/>
       <c r="B57" s="21"/>
       <c r="C57" s="20"/>
@@ -2000,7 +2139,7 @@
       <c r="I57" s="21"/>
       <c r="J57" s="20"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="20"/>
       <c r="B58" s="21"/>
       <c r="C58" s="20"/>
@@ -2012,7 +2151,7 @@
       <c r="I58" s="21"/>
       <c r="J58" s="20"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="20"/>
       <c r="B59" s="21"/>
       <c r="C59" s="20"/>
@@ -2024,7 +2163,7 @@
       <c r="I59" s="21"/>
       <c r="J59" s="20"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="20"/>
       <c r="B60" s="21"/>
       <c r="C60" s="20"/>
@@ -2036,7 +2175,7 @@
       <c r="I60" s="21"/>
       <c r="J60" s="20"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="20"/>
       <c r="B61" s="21"/>
       <c r="C61" s="20"/>
@@ -2048,7 +2187,7 @@
       <c r="I61" s="21"/>
       <c r="J61" s="20"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="20"/>
       <c r="B62" s="21"/>
       <c r="C62" s="20"/>
@@ -2060,7 +2199,7 @@
       <c r="I62" s="21"/>
       <c r="J62" s="20"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="20"/>
       <c r="B63" s="21"/>
       <c r="C63" s="20"/>
@@ -2072,7 +2211,7 @@
       <c r="I63" s="21"/>
       <c r="J63" s="20"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="20"/>
       <c r="B64" s="21"/>
       <c r="C64" s="20"/>
@@ -2084,7 +2223,7 @@
       <c r="I64" s="21"/>
       <c r="J64" s="20"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="20"/>
       <c r="B65" s="21"/>
       <c r="C65" s="20"/>
@@ -2096,7 +2235,7 @@
       <c r="I65" s="21"/>
       <c r="J65" s="20"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="20"/>
       <c r="B66" s="21"/>
       <c r="C66" s="20"/>
@@ -2108,7 +2247,7 @@
       <c r="I66" s="21"/>
       <c r="J66" s="20"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="20"/>
       <c r="B67" s="21"/>
       <c r="C67" s="20"/>
@@ -2120,7 +2259,7 @@
       <c r="I67" s="21"/>
       <c r="J67" s="20"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="20"/>
       <c r="B68" s="21"/>
       <c r="C68" s="20"/>
@@ -2132,7 +2271,7 @@
       <c r="I68" s="21"/>
       <c r="J68" s="20"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="20"/>
       <c r="B69" s="21"/>
       <c r="C69" s="20"/>
@@ -2144,7 +2283,7 @@
       <c r="I69" s="21"/>
       <c r="J69" s="20"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="20"/>
       <c r="B70" s="21"/>
       <c r="C70" s="20"/>
@@ -2156,7 +2295,7 @@
       <c r="I70" s="21"/>
       <c r="J70" s="20"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="20"/>
       <c r="B71" s="21"/>
       <c r="C71" s="20"/>
@@ -2168,7 +2307,7 @@
       <c r="I71" s="21"/>
       <c r="J71" s="20"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="20"/>
       <c r="B72" s="21"/>
       <c r="C72" s="20"/>
@@ -2180,7 +2319,7 @@
       <c r="I72" s="21"/>
       <c r="J72" s="20"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="20"/>
       <c r="B73" s="21"/>
       <c r="C73" s="20"/>
@@ -2192,7 +2331,7 @@
       <c r="I73" s="21"/>
       <c r="J73" s="20"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="20"/>
       <c r="B74" s="21"/>
       <c r="C74" s="20"/>
@@ -2204,7 +2343,7 @@
       <c r="I74" s="21"/>
       <c r="J74" s="20"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="20"/>
       <c r="B75" s="21"/>
       <c r="C75" s="20"/>
@@ -2216,7 +2355,7 @@
       <c r="I75" s="21"/>
       <c r="J75" s="20"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="20"/>
       <c r="B76" s="21"/>
       <c r="C76" s="20"/>
@@ -2228,7 +2367,7 @@
       <c r="I76" s="21"/>
       <c r="J76" s="20"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="20"/>
       <c r="B77" s="21"/>
       <c r="C77" s="20"/>
@@ -2240,7 +2379,7 @@
       <c r="I77" s="21"/>
       <c r="J77" s="20"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="20"/>
       <c r="B78" s="21"/>
       <c r="C78" s="20"/>
@@ -2252,7 +2391,7 @@
       <c r="I78" s="21"/>
       <c r="J78" s="20"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="20"/>
       <c r="B79" s="21"/>
       <c r="C79" s="20"/>
@@ -2264,7 +2403,7 @@
       <c r="I79" s="21"/>
       <c r="J79" s="20"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="20"/>
       <c r="B80" s="21"/>
       <c r="C80" s="20"/>
@@ -2276,7 +2415,7 @@
       <c r="I80" s="21"/>
       <c r="J80" s="20"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="20"/>
       <c r="B81" s="21"/>
       <c r="C81" s="20"/>
@@ -2288,7 +2427,7 @@
       <c r="I81" s="21"/>
       <c r="J81" s="20"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="20"/>
       <c r="B82" s="21"/>
       <c r="C82" s="20"/>
@@ -2300,7 +2439,7 @@
       <c r="I82" s="21"/>
       <c r="J82" s="20"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="20"/>
       <c r="B83" s="21"/>
       <c r="C83" s="20"/>
@@ -2312,7 +2451,7 @@
       <c r="I83" s="21"/>
       <c r="J83" s="20"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="20"/>
       <c r="B84" s="21"/>
       <c r="C84" s="20"/>
@@ -2324,7 +2463,7 @@
       <c r="I84" s="21"/>
       <c r="J84" s="20"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="20"/>
       <c r="B85" s="21"/>
       <c r="C85" s="20"/>
@@ -2336,7 +2475,7 @@
       <c r="I85" s="21"/>
       <c r="J85" s="20"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="20"/>
       <c r="B86" s="21"/>
       <c r="C86" s="20"/>
@@ -2348,7 +2487,7 @@
       <c r="I86" s="21"/>
       <c r="J86" s="20"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="20"/>
       <c r="B87" s="21"/>
       <c r="C87" s="20"/>
@@ -2360,7 +2499,7 @@
       <c r="I87" s="21"/>
       <c r="J87" s="20"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="20"/>
       <c r="B88" s="21"/>
       <c r="C88" s="20"/>
@@ -2372,7 +2511,7 @@
       <c r="I88" s="21"/>
       <c r="J88" s="20"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="20"/>
       <c r="B89" s="21"/>
       <c r="C89" s="20"/>
@@ -2384,7 +2523,7 @@
       <c r="I89" s="21"/>
       <c r="J89" s="20"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="20"/>
       <c r="B90" s="21"/>
       <c r="C90" s="20"/>
@@ -2396,7 +2535,7 @@
       <c r="I90" s="21"/>
       <c r="J90" s="20"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="20"/>
       <c r="B91" s="21"/>
       <c r="C91" s="20"/>
@@ -2408,7 +2547,7 @@
       <c r="I91" s="21"/>
       <c r="J91" s="20"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="20"/>
       <c r="B92" s="21"/>
       <c r="C92" s="20"/>
@@ -2420,7 +2559,7 @@
       <c r="I92" s="21"/>
       <c r="J92" s="20"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="20"/>
       <c r="B93" s="21"/>
       <c r="C93" s="20"/>
@@ -2432,7 +2571,7 @@
       <c r="I93" s="21"/>
       <c r="J93" s="20"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="20"/>
       <c r="B94" s="21"/>
       <c r="C94" s="20"/>
@@ -2444,7 +2583,7 @@
       <c r="I94" s="21"/>
       <c r="J94" s="20"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="20"/>
       <c r="B95" s="21"/>
       <c r="C95" s="20"/>
@@ -2456,7 +2595,7 @@
       <c r="I95" s="21"/>
       <c r="J95" s="20"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="20"/>
       <c r="B96" s="21"/>
       <c r="C96" s="20"/>
@@ -2468,7 +2607,7 @@
       <c r="I96" s="21"/>
       <c r="J96" s="20"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="20"/>
       <c r="B97" s="21"/>
       <c r="C97" s="20"/>
@@ -2480,7 +2619,7 @@
       <c r="I97" s="21"/>
       <c r="J97" s="20"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="20"/>
       <c r="B98" s="21"/>
       <c r="C98" s="20"/>
@@ -2492,7 +2631,7 @@
       <c r="I98" s="21"/>
       <c r="J98" s="20"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="20"/>
       <c r="B99" s="21"/>
       <c r="C99" s="20"/>
@@ -2504,7 +2643,7 @@
       <c r="I99" s="21"/>
       <c r="J99" s="20"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="20"/>
       <c r="B100" s="21"/>
       <c r="C100" s="20"/>
@@ -2516,7 +2655,7 @@
       <c r="I100" s="21"/>
       <c r="J100" s="20"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="20"/>
       <c r="B101" s="21"/>
       <c r="C101" s="20"/>
@@ -2528,7 +2667,7 @@
       <c r="I101" s="21"/>
       <c r="J101" s="20"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="20"/>
       <c r="B102" s="21"/>
       <c r="C102" s="20"/>
@@ -2540,7 +2679,7 @@
       <c r="I102" s="21"/>
       <c r="J102" s="20"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="20"/>
       <c r="B103" s="21"/>
       <c r="C103" s="20"/>
@@ -2552,7 +2691,7 @@
       <c r="I103" s="21"/>
       <c r="J103" s="20"/>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="20"/>
       <c r="B104" s="21"/>
       <c r="C104" s="20"/>
@@ -2564,7 +2703,7 @@
       <c r="I104" s="21"/>
       <c r="J104" s="20"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="20"/>
       <c r="B105" s="21"/>
       <c r="C105" s="20"/>
@@ -2576,7 +2715,7 @@
       <c r="I105" s="21"/>
       <c r="J105" s="20"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="20"/>
       <c r="B106" s="21"/>
       <c r="C106" s="20"/>
@@ -2588,7 +2727,7 @@
       <c r="I106" s="21"/>
       <c r="J106" s="20"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="20"/>
       <c r="B107" s="21"/>
       <c r="C107" s="20"/>
@@ -2600,7 +2739,7 @@
       <c r="I107" s="21"/>
       <c r="J107" s="20"/>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="20"/>
       <c r="B108" s="21"/>
       <c r="C108" s="20"/>
@@ -2612,7 +2751,7 @@
       <c r="I108" s="21"/>
       <c r="J108" s="20"/>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="20"/>
       <c r="B109" s="21"/>
       <c r="C109" s="20"/>
@@ -2624,7 +2763,7 @@
       <c r="I109" s="21"/>
       <c r="J109" s="20"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="20"/>
       <c r="B110" s="21"/>
       <c r="C110" s="20"/>
@@ -2636,7 +2775,7 @@
       <c r="I110" s="21"/>
       <c r="J110" s="20"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="20"/>
       <c r="B111" s="21"/>
       <c r="C111" s="20"/>
@@ -2648,7 +2787,7 @@
       <c r="I111" s="21"/>
       <c r="J111" s="20"/>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="20"/>
       <c r="B112" s="21"/>
       <c r="C112" s="20"/>
@@ -2660,7 +2799,7 @@
       <c r="I112" s="21"/>
       <c r="J112" s="20"/>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="20"/>
       <c r="B113" s="21"/>
       <c r="C113" s="20"/>
@@ -2672,7 +2811,7 @@
       <c r="I113" s="21"/>
       <c r="J113" s="20"/>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="20"/>
       <c r="B114" s="21"/>
       <c r="C114" s="20"/>
@@ -2684,7 +2823,7 @@
       <c r="I114" s="21"/>
       <c r="J114" s="20"/>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="20"/>
       <c r="B115" s="21"/>
       <c r="C115" s="20"/>
@@ -2696,7 +2835,7 @@
       <c r="I115" s="21"/>
       <c r="J115" s="20"/>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="20"/>
       <c r="B116" s="21"/>
       <c r="C116" s="20"/>
@@ -2708,7 +2847,7 @@
       <c r="I116" s="21"/>
       <c r="J116" s="20"/>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="20"/>
       <c r="B117" s="21"/>
       <c r="C117" s="20"/>
@@ -2720,7 +2859,7 @@
       <c r="I117" s="21"/>
       <c r="J117" s="20"/>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118" s="20"/>
       <c r="B118" s="21"/>
       <c r="C118" s="20"/>
@@ -2732,7 +2871,7 @@
       <c r="I118" s="21"/>
       <c r="J118" s="20"/>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119" s="20"/>
       <c r="B119" s="21"/>
       <c r="C119" s="20"/>
@@ -2744,7 +2883,7 @@
       <c r="I119" s="21"/>
       <c r="J119" s="20"/>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120" s="20"/>
       <c r="B120" s="21"/>
       <c r="C120" s="20"/>
@@ -2756,7 +2895,7 @@
       <c r="I120" s="21"/>
       <c r="J120" s="20"/>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121" s="20"/>
       <c r="B121" s="21"/>
       <c r="C121" s="20"/>
@@ -2768,7 +2907,7 @@
       <c r="I121" s="21"/>
       <c r="J121" s="20"/>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122" s="20"/>
       <c r="B122" s="21"/>
       <c r="C122" s="20"/>
@@ -2780,7 +2919,7 @@
       <c r="I122" s="21"/>
       <c r="J122" s="20"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123" s="20"/>
       <c r="B123" s="21"/>
       <c r="C123" s="20"/>
@@ -2792,7 +2931,7 @@
       <c r="I123" s="21"/>
       <c r="J123" s="20"/>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124" s="20"/>
       <c r="B124" s="21"/>
       <c r="C124" s="20"/>
@@ -2804,7 +2943,7 @@
       <c r="I124" s="21"/>
       <c r="J124" s="20"/>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125" s="20"/>
       <c r="B125" s="21"/>
       <c r="C125" s="20"/>
@@ -2816,7 +2955,7 @@
       <c r="I125" s="21"/>
       <c r="J125" s="20"/>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" s="20"/>
       <c r="B126" s="21"/>
       <c r="C126" s="20"/>
@@ -2828,7 +2967,7 @@
       <c r="I126" s="21"/>
       <c r="J126" s="20"/>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127" s="20"/>
       <c r="B127" s="21"/>
       <c r="C127" s="20"/>
@@ -2840,7 +2979,7 @@
       <c r="I127" s="21"/>
       <c r="J127" s="20"/>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128" s="20"/>
       <c r="B128" s="21"/>
       <c r="C128" s="20"/>
@@ -2852,7 +2991,7 @@
       <c r="I128" s="21"/>
       <c r="J128" s="20"/>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="20"/>
       <c r="B129" s="21"/>
       <c r="C129" s="20"/>
@@ -2864,7 +3003,7 @@
       <c r="I129" s="21"/>
       <c r="J129" s="20"/>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="20"/>
       <c r="B130" s="21"/>
       <c r="C130" s="20"/>
@@ -2876,7 +3015,7 @@
       <c r="I130" s="21"/>
       <c r="J130" s="20"/>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="20"/>
       <c r="B131" s="21"/>
       <c r="C131" s="20"/>
@@ -2888,7 +3027,7 @@
       <c r="I131" s="21"/>
       <c r="J131" s="20"/>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="20"/>
       <c r="B132" s="21"/>
       <c r="C132" s="20"/>
@@ -2900,7 +3039,7 @@
       <c r="I132" s="21"/>
       <c r="J132" s="20"/>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="20"/>
       <c r="B133" s="21"/>
       <c r="C133" s="20"/>
@@ -2912,7 +3051,7 @@
       <c r="I133" s="21"/>
       <c r="J133" s="20"/>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="20"/>
       <c r="B134" s="21"/>
       <c r="C134" s="20"/>
@@ -2924,7 +3063,7 @@
       <c r="I134" s="21"/>
       <c r="J134" s="20"/>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="20"/>
       <c r="B135" s="21"/>
       <c r="C135" s="20"/>
@@ -2936,7 +3075,7 @@
       <c r="I135" s="21"/>
       <c r="J135" s="20"/>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="20"/>
       <c r="B136" s="21"/>
       <c r="C136" s="20"/>
@@ -2948,7 +3087,7 @@
       <c r="I136" s="21"/>
       <c r="J136" s="20"/>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="20"/>
       <c r="B137" s="21"/>
       <c r="C137" s="20"/>
@@ -2960,7 +3099,7 @@
       <c r="I137" s="21"/>
       <c r="J137" s="20"/>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="20"/>
       <c r="B138" s="21"/>
       <c r="C138" s="20"/>
@@ -2972,7 +3111,7 @@
       <c r="I138" s="21"/>
       <c r="J138" s="20"/>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="20"/>
       <c r="B139" s="21"/>
       <c r="C139" s="20"/>
@@ -2984,7 +3123,7 @@
       <c r="I139" s="21"/>
       <c r="J139" s="20"/>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="20"/>
       <c r="B140" s="21"/>
       <c r="C140" s="20"/>
@@ -2996,7 +3135,7 @@
       <c r="I140" s="21"/>
       <c r="J140" s="20"/>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="20"/>
       <c r="B141" s="21"/>
       <c r="C141" s="20"/>
@@ -3008,7 +3147,7 @@
       <c r="I141" s="21"/>
       <c r="J141" s="20"/>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="20"/>
       <c r="B142" s="21"/>
       <c r="C142" s="20"/>
@@ -3020,7 +3159,7 @@
       <c r="I142" s="21"/>
       <c r="J142" s="20"/>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="20"/>
       <c r="B143" s="21"/>
       <c r="C143" s="20"/>
@@ -3032,7 +3171,7 @@
       <c r="I143" s="21"/>
       <c r="J143" s="20"/>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="20"/>
       <c r="B144" s="21"/>
       <c r="C144" s="20"/>
@@ -3044,7 +3183,7 @@
       <c r="I144" s="21"/>
       <c r="J144" s="20"/>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" s="20"/>
       <c r="B145" s="21"/>
       <c r="C145" s="20"/>
@@ -3056,7 +3195,7 @@
       <c r="I145" s="21"/>
       <c r="J145" s="20"/>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" s="20"/>
       <c r="B146" s="21"/>
       <c r="C146" s="20"/>
@@ -3068,7 +3207,7 @@
       <c r="I146" s="21"/>
       <c r="J146" s="20"/>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" s="20"/>
       <c r="B147" s="21"/>
       <c r="C147" s="20"/>
@@ -3080,7 +3219,7 @@
       <c r="I147" s="21"/>
       <c r="J147" s="20"/>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" s="20"/>
       <c r="B148" s="21"/>
       <c r="C148" s="20"/>
@@ -3092,7 +3231,7 @@
       <c r="I148" s="21"/>
       <c r="J148" s="20"/>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" s="20"/>
       <c r="B149" s="21"/>
       <c r="C149" s="20"/>
@@ -3104,7 +3243,7 @@
       <c r="I149" s="21"/>
       <c r="J149" s="20"/>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" s="20"/>
       <c r="B150" s="21"/>
       <c r="C150" s="20"/>
@@ -3116,7 +3255,7 @@
       <c r="I150" s="21"/>
       <c r="J150" s="20"/>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" s="20"/>
       <c r="B151" s="21"/>
       <c r="C151" s="20"/>
@@ -3128,7 +3267,7 @@
       <c r="I151" s="21"/>
       <c r="J151" s="20"/>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" s="20"/>
       <c r="B152" s="21"/>
       <c r="C152" s="20"/>
@@ -3140,7 +3279,7 @@
       <c r="I152" s="21"/>
       <c r="J152" s="20"/>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" s="20"/>
       <c r="B153" s="21"/>
       <c r="C153" s="20"/>
@@ -3152,7 +3291,7 @@
       <c r="I153" s="21"/>
       <c r="J153" s="20"/>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" s="20"/>
       <c r="B154" s="21"/>
       <c r="C154" s="20"/>
@@ -3164,7 +3303,7 @@
       <c r="I154" s="21"/>
       <c r="J154" s="20"/>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" s="20"/>
       <c r="B155" s="21"/>
       <c r="C155" s="20"/>
@@ -3176,7 +3315,7 @@
       <c r="I155" s="21"/>
       <c r="J155" s="20"/>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" s="20"/>
       <c r="B156" s="21"/>
       <c r="C156" s="20"/>
@@ -3188,7 +3327,7 @@
       <c r="I156" s="21"/>
       <c r="J156" s="20"/>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" s="20"/>
       <c r="B157" s="21"/>
       <c r="C157" s="20"/>
@@ -3200,7 +3339,7 @@
       <c r="I157" s="21"/>
       <c r="J157" s="20"/>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" s="20"/>
       <c r="B158" s="21"/>
       <c r="C158" s="20"/>
@@ -3212,7 +3351,7 @@
       <c r="I158" s="21"/>
       <c r="J158" s="20"/>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" s="20"/>
       <c r="B159" s="21"/>
       <c r="C159" s="20"/>
@@ -3224,7 +3363,7 @@
       <c r="I159" s="21"/>
       <c r="J159" s="20"/>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" s="20"/>
       <c r="B160" s="21"/>
       <c r="C160" s="20"/>
@@ -3236,7 +3375,7 @@
       <c r="I160" s="21"/>
       <c r="J160" s="20"/>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" s="20"/>
       <c r="B161" s="21"/>
       <c r="C161" s="20"/>
@@ -3248,7 +3387,7 @@
       <c r="I161" s="21"/>
       <c r="J161" s="20"/>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" s="20"/>
       <c r="B162" s="21"/>
       <c r="C162" s="20"/>
@@ -3260,7 +3399,7 @@
       <c r="I162" s="21"/>
       <c r="J162" s="20"/>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" s="20"/>
       <c r="B163" s="21"/>
       <c r="C163" s="20"/>
@@ -3272,7 +3411,7 @@
       <c r="I163" s="21"/>
       <c r="J163" s="20"/>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" s="20"/>
       <c r="B164" s="21"/>
       <c r="C164" s="20"/>
@@ -3284,7 +3423,7 @@
       <c r="I164" s="21"/>
       <c r="J164" s="20"/>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" s="20"/>
       <c r="B165" s="21"/>
       <c r="C165" s="20"/>
@@ -3296,7 +3435,7 @@
       <c r="I165" s="21"/>
       <c r="J165" s="20"/>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="20"/>
       <c r="B166" s="21"/>
       <c r="C166" s="20"/>
@@ -3308,7 +3447,7 @@
       <c r="I166" s="21"/>
       <c r="J166" s="20"/>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="20"/>
       <c r="B167" s="21"/>
       <c r="C167" s="20"/>
@@ -3320,7 +3459,7 @@
       <c r="I167" s="21"/>
       <c r="J167" s="20"/>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" s="20"/>
       <c r="B168" s="21"/>
       <c r="C168" s="20"/>
@@ -3332,7 +3471,7 @@
       <c r="I168" s="21"/>
       <c r="J168" s="20"/>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" s="20"/>
       <c r="B169" s="21"/>
       <c r="C169" s="20"/>
@@ -3344,7 +3483,7 @@
       <c r="I169" s="21"/>
       <c r="J169" s="20"/>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="20"/>
       <c r="B170" s="21"/>
       <c r="C170" s="20"/>
@@ -3356,7 +3495,7 @@
       <c r="I170" s="21"/>
       <c r="J170" s="20"/>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" s="20"/>
       <c r="B171" s="21"/>
       <c r="C171" s="20"/>
@@ -3368,7 +3507,7 @@
       <c r="I171" s="21"/>
       <c r="J171" s="20"/>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" s="20"/>
       <c r="B172" s="21"/>
       <c r="C172" s="20"/>
@@ -3380,7 +3519,7 @@
       <c r="I172" s="21"/>
       <c r="J172" s="20"/>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" s="20"/>
       <c r="B173" s="21"/>
       <c r="C173" s="20"/>
@@ -3392,7 +3531,7 @@
       <c r="I173" s="21"/>
       <c r="J173" s="20"/>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" s="20"/>
       <c r="B174" s="21"/>
       <c r="C174" s="20"/>
@@ -3404,7 +3543,7 @@
       <c r="I174" s="21"/>
       <c r="J174" s="20"/>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" s="20"/>
       <c r="B175" s="21"/>
       <c r="C175" s="20"/>
@@ -3416,7 +3555,7 @@
       <c r="I175" s="21"/>
       <c r="J175" s="20"/>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" s="20"/>
       <c r="B176" s="21"/>
       <c r="C176" s="20"/>
@@ -3428,7 +3567,7 @@
       <c r="I176" s="21"/>
       <c r="J176" s="20"/>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" s="20"/>
       <c r="B177" s="21"/>
       <c r="C177" s="20"/>
@@ -3440,7 +3579,7 @@
       <c r="I177" s="21"/>
       <c r="J177" s="20"/>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" s="20"/>
       <c r="B178" s="21"/>
       <c r="C178" s="20"/>
@@ -3452,7 +3591,7 @@
       <c r="I178" s="21"/>
       <c r="J178" s="20"/>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" s="20"/>
       <c r="B179" s="21"/>
       <c r="C179" s="20"/>
@@ -3464,7 +3603,7 @@
       <c r="I179" s="21"/>
       <c r="J179" s="20"/>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" s="20"/>
       <c r="B180" s="21"/>
       <c r="C180" s="20"/>
@@ -3476,7 +3615,7 @@
       <c r="I180" s="21"/>
       <c r="J180" s="20"/>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" s="20"/>
       <c r="B181" s="21"/>
       <c r="C181" s="20"/>
@@ -3488,7 +3627,7 @@
       <c r="I181" s="21"/>
       <c r="J181" s="20"/>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" s="20"/>
       <c r="B182" s="21"/>
       <c r="C182" s="20"/>
@@ -3500,7 +3639,7 @@
       <c r="I182" s="21"/>
       <c r="J182" s="20"/>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" s="20"/>
       <c r="B183" s="21"/>
       <c r="C183" s="20"/>
@@ -3512,7 +3651,7 @@
       <c r="I183" s="21"/>
       <c r="J183" s="20"/>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" s="20"/>
       <c r="B184" s="21"/>
       <c r="C184" s="20"/>
@@ -3524,7 +3663,7 @@
       <c r="I184" s="21"/>
       <c r="J184" s="20"/>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" s="20"/>
       <c r="B185" s="21"/>
       <c r="C185" s="20"/>
@@ -3536,7 +3675,7 @@
       <c r="I185" s="21"/>
       <c r="J185" s="20"/>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="20"/>
       <c r="B186" s="21"/>
       <c r="C186" s="20"/>
@@ -3548,7 +3687,7 @@
       <c r="I186" s="21"/>
       <c r="J186" s="20"/>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="20"/>
       <c r="B187" s="21"/>
       <c r="C187" s="20"/>
@@ -3560,7 +3699,7 @@
       <c r="I187" s="21"/>
       <c r="J187" s="20"/>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="20"/>
       <c r="B188" s="21"/>
       <c r="C188" s="20"/>
@@ -3572,7 +3711,7 @@
       <c r="I188" s="21"/>
       <c r="J188" s="20"/>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" s="20"/>
       <c r="B189" s="21"/>
       <c r="C189" s="20"/>
@@ -3584,7 +3723,7 @@
       <c r="I189" s="21"/>
       <c r="J189" s="20"/>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" s="20"/>
       <c r="B190" s="21"/>
       <c r="C190" s="20"/>
@@ -3596,7 +3735,7 @@
       <c r="I190" s="21"/>
       <c r="J190" s="20"/>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="20"/>
       <c r="B191" s="21"/>
       <c r="C191" s="20"/>
@@ -3608,7 +3747,7 @@
       <c r="I191" s="21"/>
       <c r="J191" s="20"/>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" s="20"/>
       <c r="B192" s="21"/>
       <c r="C192" s="20"/>
@@ -3620,7 +3759,7 @@
       <c r="I192" s="21"/>
       <c r="J192" s="20"/>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" s="20"/>
       <c r="B193" s="21"/>
       <c r="C193" s="20"/>
@@ -3632,7 +3771,7 @@
       <c r="I193" s="21"/>
       <c r="J193" s="20"/>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" s="20"/>
       <c r="B194" s="21"/>
       <c r="C194" s="20"/>
@@ -3644,7 +3783,7 @@
       <c r="I194" s="21"/>
       <c r="J194" s="20"/>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" s="20"/>
       <c r="B195" s="21"/>
       <c r="C195" s="20"/>
@@ -3656,7 +3795,7 @@
       <c r="I195" s="21"/>
       <c r="J195" s="20"/>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" s="20"/>
       <c r="B196" s="21"/>
       <c r="C196" s="20"/>
@@ -3668,7 +3807,7 @@
       <c r="I196" s="21"/>
       <c r="J196" s="20"/>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197" s="20"/>
       <c r="B197" s="21"/>
       <c r="C197" s="20"/>
@@ -3680,7 +3819,7 @@
       <c r="I197" s="21"/>
       <c r="J197" s="20"/>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" s="20"/>
       <c r="B198" s="21"/>
       <c r="C198" s="20"/>
@@ -3692,7 +3831,7 @@
       <c r="I198" s="21"/>
       <c r="J198" s="20"/>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" s="20"/>
       <c r="B199" s="21"/>
       <c r="C199" s="20"/>
@@ -3704,7 +3843,7 @@
       <c r="I199" s="21"/>
       <c r="J199" s="20"/>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" s="20"/>
       <c r="B200" s="21"/>
       <c r="C200" s="20"/>
@@ -3716,7 +3855,7 @@
       <c r="I200" s="21"/>
       <c r="J200" s="20"/>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" s="20"/>
       <c r="B201" s="21"/>
       <c r="C201" s="20"/>
@@ -3728,7 +3867,7 @@
       <c r="I201" s="21"/>
       <c r="J201" s="20"/>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" s="20"/>
       <c r="B202" s="21"/>
       <c r="C202" s="20"/>
@@ -3740,7 +3879,7 @@
       <c r="I202" s="21"/>
       <c r="J202" s="20"/>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" s="20"/>
       <c r="B203" s="21"/>
       <c r="C203" s="20"/>
@@ -3752,7 +3891,7 @@
       <c r="I203" s="21"/>
       <c r="J203" s="20"/>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" s="20"/>
       <c r="B204" s="21"/>
       <c r="C204" s="20"/>
@@ -3764,7 +3903,7 @@
       <c r="I204" s="21"/>
       <c r="J204" s="20"/>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" s="20"/>
       <c r="B205" s="21"/>
       <c r="C205" s="20"/>
@@ -3776,7 +3915,7 @@
       <c r="I205" s="21"/>
       <c r="J205" s="20"/>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" s="20"/>
       <c r="B206" s="21"/>
       <c r="C206" s="20"/>
@@ -3788,7 +3927,7 @@
       <c r="I206" s="21"/>
       <c r="J206" s="20"/>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" s="20"/>
       <c r="B207" s="21"/>
       <c r="C207" s="20"/>
@@ -3800,7 +3939,7 @@
       <c r="I207" s="21"/>
       <c r="J207" s="20"/>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" s="20"/>
       <c r="B208" s="21"/>
       <c r="C208" s="20"/>
@@ -3812,7 +3951,7 @@
       <c r="I208" s="21"/>
       <c r="J208" s="20"/>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209" s="20"/>
       <c r="B209" s="21"/>
       <c r="C209" s="20"/>
@@ -3824,7 +3963,7 @@
       <c r="I209" s="21"/>
       <c r="J209" s="20"/>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210" s="20"/>
       <c r="B210" s="21"/>
       <c r="C210" s="20"/>
@@ -3836,7 +3975,7 @@
       <c r="I210" s="21"/>
       <c r="J210" s="20"/>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211" s="20"/>
       <c r="B211" s="21"/>
       <c r="C211" s="20"/>
@@ -3848,7 +3987,7 @@
       <c r="I211" s="21"/>
       <c r="J211" s="20"/>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" s="20"/>
       <c r="B212" s="21"/>
       <c r="C212" s="20"/>
@@ -3860,7 +3999,7 @@
       <c r="I212" s="21"/>
       <c r="J212" s="20"/>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213" s="20"/>
       <c r="B213" s="21"/>
       <c r="C213" s="20"/>
@@ -3872,7 +4011,7 @@
       <c r="I213" s="21"/>
       <c r="J213" s="20"/>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" s="20"/>
       <c r="B214" s="21"/>
       <c r="C214" s="20"/>
@@ -3884,7 +4023,7 @@
       <c r="I214" s="21"/>
       <c r="J214" s="20"/>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215" s="20"/>
       <c r="B215" s="21"/>
       <c r="C215" s="20"/>
@@ -3896,7 +4035,7 @@
       <c r="I215" s="21"/>
       <c r="J215" s="20"/>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" s="20"/>
       <c r="B216" s="21"/>
       <c r="C216" s="20"/>
@@ -3908,7 +4047,7 @@
       <c r="I216" s="21"/>
       <c r="J216" s="20"/>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217" s="20"/>
       <c r="B217" s="21"/>
       <c r="C217" s="20"/>
@@ -3920,7 +4059,7 @@
       <c r="I217" s="21"/>
       <c r="J217" s="20"/>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" s="20"/>
       <c r="B218" s="21"/>
       <c r="C218" s="20"/>
@@ -3932,7 +4071,7 @@
       <c r="I218" s="21"/>
       <c r="J218" s="20"/>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219" s="20"/>
       <c r="B219" s="21"/>
       <c r="C219" s="20"/>
@@ -3944,7 +4083,7 @@
       <c r="I219" s="21"/>
       <c r="J219" s="20"/>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220" s="20"/>
       <c r="B220" s="21"/>
       <c r="C220" s="20"/>
@@ -3956,7 +4095,7 @@
       <c r="I220" s="21"/>
       <c r="J220" s="20"/>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221" s="20"/>
       <c r="B221" s="21"/>
       <c r="C221" s="20"/>
@@ -3968,7 +4107,7 @@
       <c r="I221" s="21"/>
       <c r="J221" s="20"/>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" s="20"/>
       <c r="B222" s="21"/>
       <c r="C222" s="20"/>
@@ -3980,7 +4119,7 @@
       <c r="I222" s="21"/>
       <c r="J222" s="20"/>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223" s="20"/>
       <c r="B223" s="21"/>
       <c r="C223" s="20"/>
@@ -3992,7 +4131,7 @@
       <c r="I223" s="21"/>
       <c r="J223" s="20"/>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224" s="20"/>
       <c r="B224" s="21"/>
       <c r="C224" s="20"/>
@@ -4004,7 +4143,7 @@
       <c r="I224" s="21"/>
       <c r="J224" s="20"/>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225" s="20"/>
       <c r="B225" s="21"/>
       <c r="C225" s="20"/>
@@ -4016,7 +4155,7 @@
       <c r="I225" s="21"/>
       <c r="J225" s="20"/>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" s="20"/>
       <c r="B226" s="21"/>
       <c r="C226" s="20"/>
@@ -4028,7 +4167,7 @@
       <c r="I226" s="21"/>
       <c r="J226" s="20"/>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227" s="20"/>
       <c r="B227" s="21"/>
       <c r="C227" s="20"/>
@@ -4040,7 +4179,7 @@
       <c r="I227" s="21"/>
       <c r="J227" s="20"/>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" s="20"/>
       <c r="B228" s="21"/>
       <c r="C228" s="20"/>
@@ -4052,7 +4191,7 @@
       <c r="I228" s="21"/>
       <c r="J228" s="20"/>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229" s="20"/>
       <c r="B229" s="21"/>
       <c r="C229" s="20"/>
@@ -4064,7 +4203,7 @@
       <c r="I229" s="21"/>
       <c r="J229" s="20"/>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" s="20"/>
       <c r="B230" s="21"/>
       <c r="C230" s="20"/>
@@ -4076,7 +4215,7 @@
       <c r="I230" s="21"/>
       <c r="J230" s="20"/>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" s="20"/>
       <c r="B231" s="21"/>
       <c r="C231" s="20"/>
@@ -4088,7 +4227,7 @@
       <c r="I231" s="21"/>
       <c r="J231" s="20"/>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" s="20"/>
       <c r="B232" s="21"/>
       <c r="C232" s="20"/>
@@ -4100,7 +4239,7 @@
       <c r="I232" s="21"/>
       <c r="J232" s="20"/>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" s="20"/>
       <c r="B233" s="21"/>
       <c r="C233" s="20"/>
@@ -4112,7 +4251,7 @@
       <c r="I233" s="21"/>
       <c r="J233" s="20"/>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" s="20"/>
       <c r="B234" s="21"/>
       <c r="C234" s="20"/>
@@ -4124,7 +4263,7 @@
       <c r="I234" s="21"/>
       <c r="J234" s="20"/>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235" s="20"/>
       <c r="B235" s="21"/>
       <c r="C235" s="20"/>
@@ -4136,7 +4275,7 @@
       <c r="I235" s="21"/>
       <c r="J235" s="20"/>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" s="20"/>
       <c r="B236" s="21"/>
       <c r="C236" s="20"/>
@@ -4148,7 +4287,7 @@
       <c r="I236" s="21"/>
       <c r="J236" s="20"/>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" s="20"/>
       <c r="B237" s="21"/>
       <c r="C237" s="20"/>
@@ -4160,7 +4299,7 @@
       <c r="I237" s="21"/>
       <c r="J237" s="20"/>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" s="20"/>
       <c r="B238" s="21"/>
       <c r="C238" s="20"/>
@@ -4172,7 +4311,7 @@
       <c r="I238" s="21"/>
       <c r="J238" s="20"/>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239" s="20"/>
       <c r="B239" s="21"/>
       <c r="C239" s="20"/>
@@ -4184,7 +4323,7 @@
       <c r="I239" s="21"/>
       <c r="J239" s="20"/>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" s="20"/>
       <c r="B240" s="21"/>
       <c r="C240" s="20"/>
@@ -4196,7 +4335,7 @@
       <c r="I240" s="21"/>
       <c r="J240" s="20"/>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" s="20"/>
       <c r="B241" s="21"/>
       <c r="C241" s="20"/>
@@ -4208,7 +4347,7 @@
       <c r="I241" s="21"/>
       <c r="J241" s="20"/>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" s="20"/>
       <c r="B242" s="21"/>
       <c r="C242" s="20"/>
@@ -4220,7 +4359,7 @@
       <c r="I242" s="21"/>
       <c r="J242" s="20"/>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243" s="20"/>
       <c r="B243" s="21"/>
       <c r="C243" s="20"/>
@@ -4232,7 +4371,7 @@
       <c r="I243" s="21"/>
       <c r="J243" s="20"/>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244" s="20"/>
       <c r="B244" s="21"/>
       <c r="C244" s="20"/>
@@ -4244,7 +4383,7 @@
       <c r="I244" s="21"/>
       <c r="J244" s="20"/>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245" s="20"/>
       <c r="B245" s="21"/>
       <c r="C245" s="20"/>
@@ -4256,7 +4395,7 @@
       <c r="I245" s="21"/>
       <c r="J245" s="20"/>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" s="20"/>
       <c r="B246" s="21"/>
       <c r="C246" s="20"/>
@@ -4268,7 +4407,7 @@
       <c r="I246" s="21"/>
       <c r="J246" s="20"/>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247" s="20"/>
       <c r="B247" s="21"/>
       <c r="C247" s="20"/>
@@ -4280,7 +4419,7 @@
       <c r="I247" s="21"/>
       <c r="J247" s="20"/>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" s="20"/>
       <c r="B248" s="21"/>
       <c r="C248" s="20"/>
@@ -4292,7 +4431,7 @@
       <c r="I248" s="21"/>
       <c r="J248" s="20"/>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249" s="20"/>
       <c r="B249" s="21"/>
       <c r="C249" s="20"/>
@@ -4304,7 +4443,7 @@
       <c r="I249" s="21"/>
       <c r="J249" s="20"/>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" s="20"/>
       <c r="B250" s="21"/>
       <c r="C250" s="20"/>
@@ -4316,7 +4455,7 @@
       <c r="I250" s="21"/>
       <c r="J250" s="20"/>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" s="20"/>
       <c r="B251" s="21"/>
       <c r="C251" s="20"/>
@@ -4328,7 +4467,7 @@
       <c r="I251" s="21"/>
       <c r="J251" s="20"/>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252" s="20"/>
       <c r="B252" s="21"/>
       <c r="C252" s="20"/>
@@ -4340,7 +4479,7 @@
       <c r="I252" s="21"/>
       <c r="J252" s="20"/>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253" s="20"/>
       <c r="B253" s="21"/>
       <c r="C253" s="20"/>
@@ -4352,7 +4491,7 @@
       <c r="I253" s="21"/>
       <c r="J253" s="20"/>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254" s="20"/>
       <c r="B254" s="21"/>
       <c r="C254" s="20"/>
@@ -4364,7 +4503,7 @@
       <c r="I254" s="21"/>
       <c r="J254" s="20"/>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255" s="20"/>
       <c r="B255" s="21"/>
       <c r="C255" s="20"/>
@@ -4376,7 +4515,7 @@
       <c r="I255" s="21"/>
       <c r="J255" s="20"/>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" s="20"/>
       <c r="B256" s="21"/>
       <c r="C256" s="20"/>
@@ -4388,7 +4527,7 @@
       <c r="I256" s="21"/>
       <c r="J256" s="20"/>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257" s="20"/>
       <c r="B257" s="21"/>
       <c r="C257" s="20"/>
@@ -4400,7 +4539,7 @@
       <c r="I257" s="21"/>
       <c r="J257" s="20"/>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" s="20"/>
       <c r="B258" s="21"/>
       <c r="C258" s="20"/>
@@ -4412,7 +4551,7 @@
       <c r="I258" s="21"/>
       <c r="J258" s="20"/>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259" s="20"/>
       <c r="B259" s="21"/>
       <c r="C259" s="20"/>
@@ -4424,7 +4563,7 @@
       <c r="I259" s="21"/>
       <c r="J259" s="20"/>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" s="20"/>
       <c r="B260" s="21"/>
       <c r="C260" s="20"/>
@@ -4436,7 +4575,7 @@
       <c r="I260" s="21"/>
       <c r="J260" s="20"/>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261" s="20"/>
       <c r="B261" s="21"/>
       <c r="C261" s="20"/>
@@ -4448,7 +4587,7 @@
       <c r="I261" s="21"/>
       <c r="J261" s="20"/>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" s="20"/>
       <c r="B262" s="21"/>
       <c r="C262" s="20"/>
@@ -4460,7 +4599,7 @@
       <c r="I262" s="21"/>
       <c r="J262" s="20"/>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263" s="20"/>
       <c r="B263" s="21"/>
       <c r="C263" s="20"/>
@@ -4472,7 +4611,7 @@
       <c r="I263" s="21"/>
       <c r="J263" s="20"/>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264" s="20"/>
       <c r="B264" s="21"/>
       <c r="C264" s="20"/>
@@ -4484,7 +4623,7 @@
       <c r="I264" s="21"/>
       <c r="J264" s="20"/>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265" s="20"/>
       <c r="B265" s="21"/>
       <c r="C265" s="20"/>
@@ -4496,7 +4635,7 @@
       <c r="I265" s="21"/>
       <c r="J265" s="20"/>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266" s="20"/>
       <c r="B266" s="21"/>
       <c r="C266" s="20"/>
@@ -4508,7 +4647,7 @@
       <c r="I266" s="21"/>
       <c r="J266" s="20"/>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267" s="20"/>
       <c r="B267" s="21"/>
       <c r="C267" s="20"/>
@@ -4520,7 +4659,7 @@
       <c r="I267" s="21"/>
       <c r="J267" s="20"/>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268" s="20"/>
       <c r="B268" s="21"/>
       <c r="C268" s="20"/>
@@ -4532,7 +4671,7 @@
       <c r="I268" s="21"/>
       <c r="J268" s="20"/>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269" s="20"/>
       <c r="B269" s="21"/>
       <c r="C269" s="20"/>
@@ -4544,7 +4683,7 @@
       <c r="I269" s="21"/>
       <c r="J269" s="20"/>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" s="20"/>
       <c r="B270" s="21"/>
       <c r="C270" s="20"/>
@@ -4556,7 +4695,7 @@
       <c r="I270" s="21"/>
       <c r="J270" s="20"/>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271" s="20"/>
       <c r="B271" s="21"/>
       <c r="C271" s="20"/>
@@ -4568,7 +4707,7 @@
       <c r="I271" s="21"/>
       <c r="J271" s="20"/>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272" s="20"/>
       <c r="B272" s="21"/>
       <c r="C272" s="20"/>
@@ -4580,7 +4719,7 @@
       <c r="I272" s="21"/>
       <c r="J272" s="20"/>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273" s="20"/>
       <c r="B273" s="21"/>
       <c r="C273" s="20"/>
@@ -4592,7 +4731,7 @@
       <c r="I273" s="21"/>
       <c r="J273" s="20"/>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274" s="20"/>
       <c r="B274" s="21"/>
       <c r="C274" s="20"/>
@@ -4604,7 +4743,7 @@
       <c r="I274" s="21"/>
       <c r="J274" s="20"/>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275" s="20"/>
       <c r="B275" s="21"/>
       <c r="C275" s="20"/>
@@ -4616,7 +4755,7 @@
       <c r="I275" s="21"/>
       <c r="J275" s="20"/>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276" s="20"/>
       <c r="B276" s="21"/>
       <c r="C276" s="20"/>
@@ -4628,7 +4767,7 @@
       <c r="I276" s="21"/>
       <c r="J276" s="20"/>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277" s="20"/>
       <c r="B277" s="21"/>
       <c r="C277" s="20"/>
@@ -4640,7 +4779,7 @@
       <c r="I277" s="21"/>
       <c r="J277" s="20"/>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278" s="20"/>
       <c r="B278" s="21"/>
       <c r="C278" s="20"/>
@@ -4652,7 +4791,7 @@
       <c r="I278" s="21"/>
       <c r="J278" s="20"/>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279" s="20"/>
       <c r="B279" s="21"/>
       <c r="C279" s="20"/>
@@ -4664,7 +4803,7 @@
       <c r="I279" s="21"/>
       <c r="J279" s="20"/>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280" s="20"/>
       <c r="B280" s="21"/>
       <c r="C280" s="20"/>
@@ -4676,7 +4815,7 @@
       <c r="I280" s="21"/>
       <c r="J280" s="20"/>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281" s="20"/>
       <c r="B281" s="21"/>
       <c r="C281" s="20"/>
@@ -4688,7 +4827,7 @@
       <c r="I281" s="21"/>
       <c r="J281" s="20"/>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282" s="20"/>
       <c r="B282" s="21"/>
       <c r="C282" s="20"/>
@@ -4700,7 +4839,7 @@
       <c r="I282" s="21"/>
       <c r="J282" s="20"/>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283" s="20"/>
       <c r="B283" s="21"/>
       <c r="C283" s="20"/>
@@ -4712,7 +4851,7 @@
       <c r="I283" s="21"/>
       <c r="J283" s="20"/>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284" s="20"/>
       <c r="B284" s="21"/>
       <c r="C284" s="20"/>
@@ -4724,7 +4863,7 @@
       <c r="I284" s="21"/>
       <c r="J284" s="20"/>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285" s="20"/>
       <c r="B285" s="21"/>
       <c r="C285" s="20"/>
@@ -4736,7 +4875,7 @@
       <c r="I285" s="21"/>
       <c r="J285" s="20"/>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286" s="20"/>
       <c r="B286" s="21"/>
       <c r="C286" s="20"/>
@@ -4748,7 +4887,7 @@
       <c r="I286" s="21"/>
       <c r="J286" s="20"/>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A287" s="20"/>
       <c r="B287" s="21"/>
       <c r="C287" s="20"/>
@@ -4760,7 +4899,7 @@
       <c r="I287" s="21"/>
       <c r="J287" s="20"/>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288" s="20"/>
       <c r="B288" s="21"/>
       <c r="C288" s="20"/>
@@ -4772,7 +4911,7 @@
       <c r="I288" s="21"/>
       <c r="J288" s="20"/>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289" s="20"/>
       <c r="B289" s="21"/>
       <c r="C289" s="20"/>
@@ -4784,7 +4923,7 @@
       <c r="I289" s="21"/>
       <c r="J289" s="20"/>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290" s="20"/>
       <c r="B290" s="21"/>
       <c r="C290" s="20"/>
@@ -4796,7 +4935,7 @@
       <c r="I290" s="21"/>
       <c r="J290" s="20"/>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291" s="20"/>
       <c r="B291" s="21"/>
       <c r="C291" s="20"/>
@@ -4808,7 +4947,7 @@
       <c r="I291" s="21"/>
       <c r="J291" s="20"/>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292" s="20"/>
       <c r="B292" s="21"/>
       <c r="C292" s="20"/>
@@ -4820,7 +4959,7 @@
       <c r="I292" s="21"/>
       <c r="J292" s="20"/>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A293" s="20"/>
       <c r="B293" s="21"/>
       <c r="C293" s="20"/>
@@ -4832,7 +4971,7 @@
       <c r="I293" s="21"/>
       <c r="J293" s="20"/>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294" s="20"/>
       <c r="B294" s="21"/>
       <c r="C294" s="20"/>
@@ -4844,7 +4983,7 @@
       <c r="I294" s="21"/>
       <c r="J294" s="20"/>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295" s="20"/>
       <c r="B295" s="21"/>
       <c r="C295" s="20"/>
@@ -4856,7 +4995,7 @@
       <c r="I295" s="21"/>
       <c r="J295" s="20"/>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296" s="20"/>
       <c r="B296" s="21"/>
       <c r="C296" s="20"/>
@@ -4868,7 +5007,7 @@
       <c r="I296" s="21"/>
       <c r="J296" s="20"/>
     </row>
-    <row r="297" spans="1:10">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297" s="20"/>
       <c r="B297" s="21"/>
       <c r="C297" s="20"/>
@@ -4880,7 +5019,7 @@
       <c r="I297" s="21"/>
       <c r="J297" s="20"/>
     </row>
-    <row r="298" spans="1:10">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298" s="20"/>
       <c r="B298" s="21"/>
       <c r="C298" s="20"/>
@@ -4892,7 +5031,7 @@
       <c r="I298" s="21"/>
       <c r="J298" s="20"/>
     </row>
-    <row r="299" spans="1:10">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299" s="20"/>
       <c r="B299" s="21"/>
       <c r="C299" s="20"/>
@@ -4904,7 +5043,7 @@
       <c r="I299" s="21"/>
       <c r="J299" s="20"/>
     </row>
-    <row r="300" spans="1:10">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300" s="20"/>
       <c r="B300" s="21"/>
       <c r="C300" s="20"/>
@@ -4916,7 +5055,7 @@
       <c r="I300" s="21"/>
       <c r="J300" s="20"/>
     </row>
-    <row r="301" spans="1:10">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301" s="20"/>
       <c r="B301" s="21"/>
       <c r="C301" s="20"/>
@@ -4928,7 +5067,7 @@
       <c r="I301" s="21"/>
       <c r="J301" s="20"/>
     </row>
-    <row r="302" spans="1:10">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302" s="20"/>
       <c r="B302" s="21"/>
       <c r="C302" s="20"/>
@@ -4940,7 +5079,7 @@
       <c r="I302" s="21"/>
       <c r="J302" s="20"/>
     </row>
-    <row r="303" spans="1:10">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303" s="20"/>
       <c r="B303" s="21"/>
       <c r="C303" s="20"/>
@@ -4952,7 +5091,7 @@
       <c r="I303" s="21"/>
       <c r="J303" s="20"/>
     </row>
-    <row r="304" spans="1:10">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304" s="20"/>
       <c r="B304" s="21"/>
       <c r="C304" s="20"/>
@@ -4964,7 +5103,7 @@
       <c r="I304" s="21"/>
       <c r="J304" s="20"/>
     </row>
-    <row r="305" spans="1:10">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A305" s="20"/>
       <c r="B305" s="21"/>
       <c r="C305" s="20"/>
@@ -4976,7 +5115,7 @@
       <c r="I305" s="21"/>
       <c r="J305" s="20"/>
     </row>
-    <row r="306" spans="1:10">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A306" s="20"/>
       <c r="B306" s="21"/>
       <c r="C306" s="20"/>
@@ -4988,7 +5127,7 @@
       <c r="I306" s="21"/>
       <c r="J306" s="20"/>
     </row>
-    <row r="307" spans="1:10">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A307" s="20"/>
       <c r="B307" s="21"/>
       <c r="C307" s="20"/>
@@ -5000,7 +5139,7 @@
       <c r="I307" s="21"/>
       <c r="J307" s="20"/>
     </row>
-    <row r="308" spans="1:10">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A308" s="20"/>
       <c r="B308" s="21"/>
       <c r="C308" s="20"/>
@@ -5012,7 +5151,7 @@
       <c r="I308" s="21"/>
       <c r="J308" s="20"/>
     </row>
-    <row r="309" spans="1:10">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A309" s="20"/>
       <c r="B309" s="21"/>
       <c r="C309" s="20"/>
@@ -5024,7 +5163,7 @@
       <c r="I309" s="21"/>
       <c r="J309" s="20"/>
     </row>
-    <row r="310" spans="1:10">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A310" s="20"/>
       <c r="B310" s="21"/>
       <c r="C310" s="20"/>
@@ -5036,7 +5175,7 @@
       <c r="I310" s="21"/>
       <c r="J310" s="20"/>
     </row>
-    <row r="311" spans="1:10">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311" s="20"/>
       <c r="B311" s="21"/>
       <c r="C311" s="20"/>
@@ -5048,7 +5187,7 @@
       <c r="I311" s="21"/>
       <c r="J311" s="20"/>
     </row>
-    <row r="312" spans="1:10">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A312" s="20"/>
       <c r="B312" s="21"/>
       <c r="C312" s="20"/>
@@ -5060,7 +5199,7 @@
       <c r="I312" s="21"/>
       <c r="J312" s="20"/>
     </row>
-    <row r="313" spans="1:10">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A313" s="20"/>
       <c r="B313" s="21"/>
       <c r="C313" s="20"/>
@@ -5072,7 +5211,7 @@
       <c r="I313" s="21"/>
       <c r="J313" s="20"/>
     </row>
-    <row r="314" spans="1:10">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A314" s="20"/>
       <c r="B314" s="21"/>
       <c r="C314" s="20"/>
@@ -5084,7 +5223,7 @@
       <c r="I314" s="21"/>
       <c r="J314" s="20"/>
     </row>
-    <row r="315" spans="1:10">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A315" s="20"/>
       <c r="B315" s="21"/>
       <c r="C315" s="20"/>
@@ -5096,7 +5235,7 @@
       <c r="I315" s="21"/>
       <c r="J315" s="20"/>
     </row>
-    <row r="316" spans="1:10">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A316" s="20"/>
       <c r="B316" s="21"/>
       <c r="C316" s="20"/>
@@ -5108,7 +5247,7 @@
       <c r="I316" s="21"/>
       <c r="J316" s="20"/>
     </row>
-    <row r="317" spans="1:10">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A317" s="20"/>
       <c r="B317" s="21"/>
       <c r="C317" s="20"/>
@@ -5120,7 +5259,7 @@
       <c r="I317" s="21"/>
       <c r="J317" s="20"/>
     </row>
-    <row r="318" spans="1:10">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A318" s="20"/>
       <c r="B318" s="21"/>
       <c r="C318" s="20"/>
@@ -5132,7 +5271,7 @@
       <c r="I318" s="21"/>
       <c r="J318" s="20"/>
     </row>
-    <row r="319" spans="1:10">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A319" s="20"/>
       <c r="B319" s="21"/>
       <c r="C319" s="20"/>
@@ -5144,7 +5283,7 @@
       <c r="I319" s="21"/>
       <c r="J319" s="20"/>
     </row>
-    <row r="320" spans="1:10">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A320" s="20"/>
       <c r="B320" s="21"/>
       <c r="C320" s="20"/>
@@ -5156,7 +5295,7 @@
       <c r="I320" s="21"/>
       <c r="J320" s="20"/>
     </row>
-    <row r="321" spans="1:10">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A321" s="20"/>
       <c r="B321" s="21"/>
       <c r="C321" s="20"/>
@@ -5168,7 +5307,7 @@
       <c r="I321" s="21"/>
       <c r="J321" s="20"/>
     </row>
-    <row r="322" spans="1:10">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A322" s="20"/>
       <c r="B322" s="21"/>
       <c r="C322" s="20"/>
@@ -5180,7 +5319,7 @@
       <c r="I322" s="21"/>
       <c r="J322" s="20"/>
     </row>
-    <row r="323" spans="1:10">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A323" s="20"/>
       <c r="B323" s="21"/>
       <c r="C323" s="20"/>
@@ -5192,7 +5331,7 @@
       <c r="I323" s="21"/>
       <c r="J323" s="20"/>
     </row>
-    <row r="324" spans="1:10">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A324" s="20"/>
       <c r="B324" s="21"/>
       <c r="C324" s="20"/>
@@ -5204,7 +5343,7 @@
       <c r="I324" s="21"/>
       <c r="J324" s="20"/>
     </row>
-    <row r="325" spans="1:10">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A325" s="20"/>
       <c r="B325" s="21"/>
       <c r="C325" s="20"/>
@@ -5216,7 +5355,7 @@
       <c r="I325" s="21"/>
       <c r="J325" s="20"/>
     </row>
-    <row r="326" spans="1:10">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A326" s="20"/>
       <c r="B326" s="21"/>
       <c r="C326" s="20"/>
@@ -5228,7 +5367,7 @@
       <c r="I326" s="21"/>
       <c r="J326" s="20"/>
     </row>
-    <row r="327" spans="1:10">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A327" s="20"/>
       <c r="B327" s="21"/>
       <c r="C327" s="20"/>
@@ -5240,7 +5379,7 @@
       <c r="I327" s="21"/>
       <c r="J327" s="20"/>
     </row>
-    <row r="328" spans="1:10">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A328" s="20"/>
       <c r="B328" s="21"/>
       <c r="C328" s="20"/>
@@ -5252,7 +5391,7 @@
       <c r="I328" s="21"/>
       <c r="J328" s="20"/>
     </row>
-    <row r="329" spans="1:10">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A329" s="20"/>
       <c r="B329" s="21"/>
       <c r="C329" s="20"/>
@@ -5264,7 +5403,7 @@
       <c r="I329" s="21"/>
       <c r="J329" s="20"/>
     </row>
-    <row r="330" spans="1:10">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A330" s="20"/>
       <c r="B330" s="21"/>
       <c r="C330" s="20"/>
@@ -5276,7 +5415,7 @@
       <c r="I330" s="21"/>
       <c r="J330" s="20"/>
     </row>
-    <row r="331" spans="1:10">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A331" s="20"/>
       <c r="B331" s="21"/>
       <c r="C331" s="20"/>
@@ -5288,7 +5427,7 @@
       <c r="I331" s="21"/>
       <c r="J331" s="20"/>
     </row>
-    <row r="332" spans="1:10">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A332" s="20"/>
       <c r="B332" s="21"/>
       <c r="C332" s="20"/>
@@ -5300,7 +5439,7 @@
       <c r="I332" s="21"/>
       <c r="J332" s="20"/>
     </row>
-    <row r="333" spans="1:10">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A333" s="20"/>
       <c r="B333" s="21"/>
       <c r="C333" s="20"/>
@@ -5312,7 +5451,7 @@
       <c r="I333" s="21"/>
       <c r="J333" s="20"/>
     </row>
-    <row r="334" spans="1:10">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A334" s="20"/>
       <c r="B334" s="21"/>
       <c r="C334" s="20"/>
@@ -5324,7 +5463,7 @@
       <c r="I334" s="21"/>
       <c r="J334" s="20"/>
     </row>
-    <row r="335" spans="1:10">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A335" s="20"/>
       <c r="B335" s="21"/>
       <c r="C335" s="20"/>
@@ -5336,7 +5475,7 @@
       <c r="I335" s="21"/>
       <c r="J335" s="20"/>
     </row>
-    <row r="336" spans="1:10">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A336" s="20"/>
       <c r="B336" s="21"/>
       <c r="C336" s="20"/>
@@ -5348,7 +5487,7 @@
       <c r="I336" s="21"/>
       <c r="J336" s="20"/>
     </row>
-    <row r="337" spans="1:10">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337" s="20"/>
       <c r="B337" s="21"/>
       <c r="C337" s="20"/>
@@ -5360,7 +5499,7 @@
       <c r="I337" s="21"/>
       <c r="J337" s="20"/>
     </row>
-    <row r="338" spans="1:10">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338" s="20"/>
       <c r="B338" s="21"/>
       <c r="C338" s="20"/>
@@ -5372,7 +5511,7 @@
       <c r="I338" s="21"/>
       <c r="J338" s="20"/>
     </row>
-    <row r="339" spans="1:10">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A339" s="20"/>
       <c r="B339" s="21"/>
       <c r="C339" s="20"/>
@@ -5384,7 +5523,7 @@
       <c r="I339" s="21"/>
       <c r="J339" s="20"/>
     </row>
-    <row r="340" spans="1:10">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A340" s="20"/>
       <c r="B340" s="21"/>
       <c r="C340" s="20"/>
@@ -5396,7 +5535,7 @@
       <c r="I340" s="21"/>
       <c r="J340" s="20"/>
     </row>
-    <row r="341" spans="1:10">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341" s="20"/>
       <c r="B341" s="21"/>
       <c r="C341" s="20"/>
@@ -5408,7 +5547,7 @@
       <c r="I341" s="21"/>
       <c r="J341" s="20"/>
     </row>
-    <row r="342" spans="1:10">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342" s="20"/>
       <c r="B342" s="21"/>
       <c r="C342" s="20"/>
@@ -5420,7 +5559,7 @@
       <c r="I342" s="21"/>
       <c r="J342" s="20"/>
     </row>
-    <row r="343" spans="1:10">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343" s="20"/>
       <c r="B343" s="21"/>
       <c r="C343" s="20"/>
@@ -5432,7 +5571,7 @@
       <c r="I343" s="21"/>
       <c r="J343" s="20"/>
     </row>
-    <row r="344" spans="1:10">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344" s="20"/>
       <c r="B344" s="21"/>
       <c r="C344" s="20"/>
@@ -5444,7 +5583,7 @@
       <c r="I344" s="21"/>
       <c r="J344" s="20"/>
     </row>
-    <row r="345" spans="1:10">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A345" s="22"/>
       <c r="B345" s="21"/>
       <c r="C345" s="20"/>
@@ -5456,7 +5595,7 @@
       <c r="I345" s="21"/>
       <c r="J345" s="22"/>
     </row>
-    <row r="346" spans="1:10">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A346" s="22"/>
       <c r="B346" s="21"/>
       <c r="C346" s="22"/>
@@ -5468,7 +5607,7 @@
       <c r="I346" s="21"/>
       <c r="J346" s="22"/>
     </row>
-    <row r="347" spans="1:10">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347" s="22"/>
       <c r="B347" s="21"/>
       <c r="C347" s="22"/>
@@ -5480,7 +5619,7 @@
       <c r="I347" s="21"/>
       <c r="J347" s="22"/>
     </row>
-    <row r="348" spans="1:10">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348" s="22"/>
       <c r="B348" s="21"/>
       <c r="C348" s="22"/>
@@ -5492,7 +5631,7 @@
       <c r="I348" s="21"/>
       <c r="J348" s="22"/>
     </row>
-    <row r="349" spans="1:10">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A349" s="22"/>
       <c r="B349" s="21"/>
       <c r="C349" s="22"/>
@@ -5518,14 +5657,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25:J26"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
@@ -5537,8 +5676,8 @@
     <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -5559,12 +5698,12 @@
       <c r="I1" s="20"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="47.25">
-      <c r="A2" s="51"/>
+    <row r="2" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="75"/>
       <c r="B2" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="55" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="30" t="s">
@@ -5579,7 +5718,7 @@
       <c r="I2" s="20"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="35"/>
       <c r="B3" s="36" t="s">
         <v>17</v>
@@ -5597,7 +5736,7 @@
       <c r="I3" s="20"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="39"/>
       <c r="B4" s="36"/>
       <c r="C4" s="30"/>
@@ -5611,7 +5750,7 @@
       <c r="I4" s="20"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="25"/>
       <c r="B5" s="3"/>
       <c r="C5" s="2"/>
@@ -5623,37 +5762,37 @@
       <c r="I5" s="20"/>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="49"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
+      <c r="H6" s="72"/>
+      <c r="I6" s="73"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="22.5">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="71"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -5669,7 +5808,7 @@
       <c r="I8" s="27"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="13.5" thickBot="1">
+    <row r="9" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="7"/>
       <c r="C9" s="6"/>
@@ -5681,7 +5820,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5" thickBot="1">
+    <row r="10" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
         <v>18</v>
       </c>
@@ -5700,7 +5839,7 @@
       <c r="F10" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="68" t="s">
+      <c r="G10" s="59" t="s">
         <v>12</v>
       </c>
       <c r="H10" s="42" t="s">
@@ -5713,309 +5852,566 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="51">
-      <c r="A11" s="53" t="s">
+    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="53" t="s">
+      <c r="D11" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="69" t="s">
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="55"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="56"/>
-    </row>
-    <row r="12" spans="1:10" ht="38.25">
-      <c r="A12" s="57"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53" t="s">
+      <c r="H11" s="48"/>
+      <c r="I11" s="47"/>
+      <c r="J11" s="49"/>
+    </row>
+    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="50"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="60"/>
-    </row>
-    <row r="13" spans="1:10" ht="39" thickBot="1">
-      <c r="A13" s="65"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65" t="s">
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="53"/>
+    </row>
+    <row r="13" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="56"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="63"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="66"/>
-      <c r="J13" s="71"/>
-    </row>
-    <row r="14" spans="1:10" ht="51.75" thickTop="1">
-      <c r="A14" s="53" t="s">
+      <c r="G13" s="77"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="60"/>
+    </row>
+    <row r="14" spans="1:10" ht="51.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="53" t="s">
+      <c r="B14" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="69" t="s">
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="55"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="56"/>
-    </row>
-    <row r="15" spans="1:10" ht="38.25">
-      <c r="A15" s="57"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="53"/>
-      <c r="D15" s="53" t="s">
+      <c r="H14" s="48"/>
+      <c r="I14" s="47"/>
+      <c r="J14" s="49"/>
+    </row>
+    <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="50"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="60"/>
-    </row>
-    <row r="16" spans="1:10" ht="39" thickBot="1">
-      <c r="A16" s="65"/>
-      <c r="B16" s="66"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="65" t="s">
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="53"/>
+    </row>
+    <row r="16" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="56"/>
+      <c r="B16" s="57"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="67" t="s">
+      <c r="E16" s="58" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="67" t="s">
+      <c r="F16" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="63"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="71"/>
-    </row>
-    <row r="17" spans="1:13" ht="64.5" thickTop="1">
-      <c r="A17" s="53" t="s">
+      <c r="G16" s="77"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="60"/>
+    </row>
+    <row r="17" spans="1:13" ht="64.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="53" t="s">
+      <c r="C17" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="53" t="s">
+      <c r="D17" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="69" t="s">
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="55"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="56"/>
-    </row>
-    <row r="18" spans="1:13" ht="38.25">
-      <c r="A18" s="57"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53" t="s">
+      <c r="H17" s="48"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="49"/>
+    </row>
+    <row r="18" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="50"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="63"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="60"/>
-    </row>
-    <row r="19" spans="1:13" ht="38.25">
-      <c r="A19" s="57"/>
-      <c r="B19" s="58"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53" t="s">
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="53"/>
+    </row>
+    <row r="19" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="50"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="59"/>
-      <c r="G19" s="63"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="60"/>
-    </row>
-    <row r="20" spans="1:13" ht="39" thickBot="1">
-      <c r="A20" s="65"/>
-      <c r="B20" s="66"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65" t="s">
+      <c r="F19" s="52"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="53"/>
+    </row>
+    <row r="20" spans="1:13" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="56"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="67" t="s">
+      <c r="E20" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="67" t="s">
+      <c r="F20" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="70"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="71"/>
-    </row>
-    <row r="21" spans="1:13" ht="39" thickTop="1">
-      <c r="A21" s="53" t="s">
+      <c r="G20" s="78"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="60"/>
+    </row>
+    <row r="21" spans="1:13" ht="39" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="53" t="s">
+      <c r="C21" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D21" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="72" t="s">
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="55"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="56"/>
-    </row>
-    <row r="22" spans="1:13" ht="63.75">
-      <c r="A22" s="57"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53" t="s">
+      <c r="H21" s="48"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="49"/>
+    </row>
+    <row r="22" spans="1:13" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="50"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="59"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="74" t="s">
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="63" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="59"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="60"/>
-    </row>
-    <row r="23" spans="1:13" ht="53.25" customHeight="1">
-      <c r="A23" s="57"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53" t="s">
+      <c r="H22" s="52"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="53"/>
+    </row>
+    <row r="23" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="50"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="59"/>
-      <c r="G23" s="74" t="s">
+      <c r="F23" s="52"/>
+      <c r="G23" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="59"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="60"/>
-    </row>
-    <row r="24" spans="1:13" ht="95.25" customHeight="1">
-      <c r="A24" s="57"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="53" t="s">
+      <c r="H23" s="52"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="53"/>
+    </row>
+    <row r="24" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="50"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="59" t="s">
+      <c r="E24" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="F24" s="59" t="s">
+      <c r="F24" s="52" t="s">
         <v>57</v>
       </c>
-      <c r="G24" s="55" t="s">
+      <c r="G24" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="59"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="60"/>
-      <c r="L24" s="76"/>
-    </row>
-    <row r="25" spans="1:13" ht="51">
-      <c r="A25" s="75"/>
-      <c r="B25" s="77"/>
-      <c r="C25" s="82"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="55" t="s">
+      <c r="H24" s="52"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="53"/>
+      <c r="L24" s="65"/>
+    </row>
+    <row r="25" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="64"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="H25" s="75"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="77"/>
-      <c r="L25" s="62"/>
-    </row>
-    <row r="26" spans="1:13" ht="64.5" thickBot="1">
-      <c r="A26" s="78"/>
-      <c r="B26" s="79"/>
-      <c r="C26" s="83"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61" t="s">
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="66"/>
+      <c r="L25" s="54"/>
+    </row>
+    <row r="26" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="82"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="84"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="78"/>
-      <c r="I26" s="78"/>
-      <c r="J26" s="79"/>
-      <c r="L26" s="62"/>
-    </row>
-    <row r="27" spans="1:13" ht="15">
-      <c r="M27" s="73"/>
-    </row>
-    <row r="28" spans="1:13" ht="15">
-      <c r="L28" s="62"/>
-    </row>
-    <row r="29" spans="1:13" ht="15">
-      <c r="L29" s="62"/>
-    </row>
-    <row r="30" spans="1:13" ht="15">
-      <c r="M30" s="73" t="s">
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="83"/>
+      <c r="L26" s="54"/>
+    </row>
+    <row r="27" spans="1:13" ht="50.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="80" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="80"/>
+      <c r="F27" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="80"/>
+      <c r="J27" s="80"/>
+      <c r="M27" s="62"/>
+    </row>
+    <row r="28" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="64"/>
+      <c r="B28" s="64"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="64"/>
+      <c r="F28" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="64"/>
+      <c r="L28" s="54"/>
+    </row>
+    <row r="29" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="64"/>
+      <c r="B29" s="64"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="L29" s="54"/>
+    </row>
+    <row r="30" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="64"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="64"/>
+      <c r="M30" s="62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15">
-      <c r="L31" s="62" t="s">
+    <row r="31" spans="1:13" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="82"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="88" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="82"/>
+      <c r="F31" s="89" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="82"/>
+      <c r="L31" s="54" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="15">
-      <c r="L32" s="52" t="s">
+    <row r="32" spans="1:13" ht="45.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="81" t="s">
+        <v>75</v>
+      </c>
+      <c r="C32" s="90" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="93" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="80"/>
+      <c r="F32" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="L32" s="45" t="s">
         <v>61</v>
       </c>
     </row>
+    <row r="33" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="64"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="91" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="H33" s="64"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="64"/>
+    </row>
+    <row r="34" spans="1:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="82"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="92" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="82"/>
+      <c r="F34" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" s="82"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="82"/>
+      <c r="J34" s="82"/>
+    </row>
+    <row r="35" spans="1:10" ht="43.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="81" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="90" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="90" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="80"/>
+      <c r="F35" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+    </row>
+    <row r="36" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="64"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="79" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" s="64"/>
+      <c r="F36" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+    </row>
+    <row r="37" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="64"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="79" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="64"/>
+      <c r="I37" s="64"/>
+      <c r="J37" s="64"/>
+    </row>
+    <row r="38" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="64"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="64"/>
+    </row>
+    <row r="39" spans="1:10" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="82"/>
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="88" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="82"/>
+      <c r="F39" s="89" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="82"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="82"/>
+    </row>
+    <row r="40" spans="1:10" ht="39" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="81" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="81" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="90" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="90" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="80"/>
+      <c r="F40" s="90" t="s">
+        <v>95</v>
+      </c>
+      <c r="G40" s="80"/>
+      <c r="H40" s="80"/>
+      <c r="I40" s="80"/>
+      <c r="J40" s="80"/>
+    </row>
+    <row r="41" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="64"/>
+      <c r="B41" s="64"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="87" t="s">
+        <v>93</v>
+      </c>
+      <c r="E41" s="64"/>
+      <c r="F41" s="64"/>
+      <c r="G41" s="64"/>
+      <c r="H41" s="64"/>
+      <c r="I41" s="64"/>
+      <c r="J41" s="64"/>
+    </row>
+    <row r="42" spans="1:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="82"/>
+      <c r="B42" s="82"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42" s="82"/>
+      <c r="F42" s="89" t="s">
+        <v>96</v>
+      </c>
+      <c r="G42" s="82"/>
+      <c r="H42" s="82"/>
+      <c r="I42" s="82"/>
+      <c r="J42" s="82"/>
+    </row>
+    <row r="43" spans="1:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G17:G20"/>
@@ -6027,18 +6423,18 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added a test case for interest calculator
test case for intreest calculator
</commit_message>
<xml_diff>
--- a/TestCaseTemplateRBSUEljunia.xlsx
+++ b/TestCaseTemplateRBSUEljunia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
   <si>
     <t>Dependencies:</t>
   </si>
@@ -207,12 +207,6 @@
     <t>4.4.3 Authorization fails – new password and confirmed password are less than 6 chars</t>
   </si>
   <si>
-    <t>4.4.2 Allow him to re-enter and confirm new password</t>
-  </si>
-  <si>
-    <t>4.4.1 System prompts the user that password must be at least 6 characters</t>
-  </si>
-  <si>
     <t>System prompts the user that he typed the password wrong and allows him to re-enter the password</t>
   </si>
   <si>
@@ -319,6 +313,30 @@
   </si>
   <si>
     <t>TC-4.9</t>
+  </si>
+  <si>
+    <t>Test intrest calculator</t>
+  </si>
+  <si>
+    <t>Test if the interest calculator is working properly</t>
+  </si>
+  <si>
+    <t>User clicks the calculator tab in the menu</t>
+  </si>
+  <si>
+    <t>Calculator page should be displaed</t>
+  </si>
+  <si>
+    <t>Fill the fields required to calculate</t>
+  </si>
+  <si>
+    <t>Click the button calculate</t>
+  </si>
+  <si>
+    <t>Test currency field, test base amount and so on to fill the all.</t>
+  </si>
+  <si>
+    <t>Files should be secure and not able to inject scripts in the HTML forms</t>
   </si>
 </sst>
 </file>
@@ -329,7 +347,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;лв.&quot;_-;\-* #,##0.00\ &quot;лв.&quot;_-;_-* &quot;-&quot;??\ &quot;лв.&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -440,8 +458,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,8 +481,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="27">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -823,11 +855,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -957,7 +1036,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -982,9 +1060,6 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="6"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -997,42 +1072,27 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1048,6 +1108,126 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1078,8 +1258,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="30" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="3" borderId="30" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1403,7 +1596,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="114" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="29" t="s">
@@ -1425,7 +1618,7 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="90"/>
+      <c r="A2" s="115"/>
       <c r="B2" s="33" t="s">
         <v>16</v>
       </c>
@@ -1490,28 +1683,28 @@
       <c r="A6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="88"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="112"/>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="113"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="86"/>
+      <c r="B7" s="109"/>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="111"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -5656,139 +5849,140 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" style="77" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="77" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" style="77" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" style="77" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="77" customWidth="1"/>
+    <col min="6" max="6" width="18" style="77" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" style="77" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="77" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="119" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="74" t="s">
         <v>21</v>
       </c>
       <c r="F1" s="32"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="1"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="1:10" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="90"/>
-      <c r="B2" s="33" t="s">
+      <c r="A2" s="120"/>
+      <c r="B2" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="79">
         <v>42476</v>
       </c>
       <c r="F2" s="32"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="1"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="76"/>
     </row>
     <row r="3" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="36" t="s">
+      <c r="A3" s="80"/>
+      <c r="B3" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="38"/>
+      <c r="E3" s="83"/>
       <c r="F3" s="32"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="1"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="76"/>
     </row>
     <row r="4" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30" t="s">
+      <c r="A4" s="84"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="40"/>
+      <c r="E4" s="85"/>
       <c r="F4" s="32"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="1"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="76"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="2"/>
+      <c r="A5" s="86"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="88"/>
     </row>
     <row r="6" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="5"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
+      <c r="I6" s="111"/>
+      <c r="J6" s="90"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="85"/>
-      <c r="E7" s="85"/>
-      <c r="F7" s="85"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="5"/>
+      <c r="B7" s="109"/>
+      <c r="C7" s="110"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
+      <c r="H7" s="110"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="90"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -5804,672 +5998,682 @@
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
-      <c r="J8" s="5"/>
+      <c r="J8" s="90"/>
     </row>
     <row r="9" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41" t="s">
+      <c r="A9" s="91"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="93"/>
+    </row>
+    <row r="10" spans="1:10" ht="25.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="42" t="s">
+      <c r="F10" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="96" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="42" t="s">
+      <c r="H10" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="42" t="s">
+      <c r="I10" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="43" t="s">
+      <c r="J10" s="97" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="50.4" x14ac:dyDescent="0.25">
-      <c r="A11" s="46" t="s">
+    <row r="11" spans="1:10" ht="51.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="91" t="s">
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="116" t="s">
         <v>36</v>
       </c>
-      <c r="H11" s="48"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="49"/>
-    </row>
-    <row r="12" spans="1:10" ht="37.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46" t="s">
+      <c r="H11" s="47"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="48"/>
+    </row>
+    <row r="12" spans="1:10" ht="38.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="53"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="51"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="52"/>
     </row>
     <row r="13" spans="1:10" ht="38.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="56"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="56" t="s">
+      <c r="A13" s="54"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="92"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="60"/>
-    </row>
-    <row r="14" spans="1:10" ht="51" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
+      <c r="G13" s="117"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="57"/>
+    </row>
+    <row r="14" spans="1:10" ht="37.200000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="69"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="72"/>
+    </row>
+    <row r="15" spans="1:10" ht="51.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B15" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C15" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D15" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="91" t="s">
+      <c r="E15" s="47"/>
+      <c r="F15" s="47"/>
+      <c r="G15" s="116" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="48"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="49"/>
-    </row>
-    <row r="15" spans="1:10" ht="37.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A15" s="50"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46" t="s">
+      <c r="H15" s="47"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="48"/>
+    </row>
+    <row r="16" spans="1:10" ht="38.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="51"/>
-      <c r="J15" s="53"/>
-    </row>
-    <row r="16" spans="1:10" ht="38.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="56"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56" t="s">
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="117"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="52"/>
+    </row>
+    <row r="17" spans="1:13" ht="38.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="54"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E17" s="56" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="58" t="s">
+      <c r="F17" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="G16" s="92"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="60"/>
-    </row>
-    <row r="17" spans="1:13" ht="63.6" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="46" t="s">
+      <c r="G17" s="117"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="57"/>
+    </row>
+    <row r="18" spans="1:13" ht="64.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B18" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C18" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D18" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="91" t="s">
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="116" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="48"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="49"/>
-    </row>
-    <row r="18" spans="1:13" ht="37.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A18" s="50"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46" t="s">
+      <c r="H18" s="47"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="48"/>
+    </row>
+    <row r="19" spans="1:13" ht="38.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="49"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="92"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="53"/>
-    </row>
-    <row r="19" spans="1:13" ht="37.799999999999997" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46" t="s">
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="117"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="52"/>
+    </row>
+    <row r="20" spans="1:13" ht="37.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="92"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="53"/>
-    </row>
-    <row r="20" spans="1:13" ht="38.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="56"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56" t="s">
+      <c r="F20" s="51"/>
+      <c r="G20" s="117"/>
+      <c r="H20" s="51"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="52"/>
+    </row>
+    <row r="21" spans="1:13" ht="38.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="54"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="58" t="s">
+      <c r="E21" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="F20" s="58" t="s">
+      <c r="F21" s="56" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="93"/>
-      <c r="H20" s="58"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="60"/>
-    </row>
-    <row r="21" spans="1:13" ht="38.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="G21" s="118"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="55"/>
+      <c r="J21" s="57"/>
+    </row>
+    <row r="22" spans="1:13" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B22" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C22" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D22" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="61" t="s">
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="48"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="49"/>
-    </row>
-    <row r="22" spans="1:13" ht="63" x14ac:dyDescent="0.25">
-      <c r="A22" s="50"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46" t="s">
+      <c r="H22" s="47"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="48"/>
+    </row>
+    <row r="23" spans="1:13" ht="63.6" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="49"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="63" t="s">
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="51"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="52"/>
+    </row>
+    <row r="24" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="F24" s="51"/>
+      <c r="G24" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="51"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="52"/>
+    </row>
+    <row r="25" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="49"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="51" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="H25" s="51"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="52"/>
+      <c r="L25" s="60"/>
+    </row>
+    <row r="26" spans="1:13" ht="50.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="98"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="98"/>
+      <c r="I26" s="98"/>
+      <c r="J26" s="99"/>
+      <c r="L26" s="102"/>
+    </row>
+    <row r="27" spans="1:13" ht="63.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="103"/>
+      <c r="B27" s="104"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="106"/>
+      <c r="E27" s="103"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="52"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="53"/>
-    </row>
-    <row r="23" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="52"/>
-      <c r="G23" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" s="52"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="53"/>
-    </row>
-    <row r="24" spans="1:13" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="50"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="48" t="s">
+      <c r="H27" s="103"/>
+      <c r="I27" s="103"/>
+      <c r="J27" s="104"/>
+      <c r="L27" s="102"/>
+    </row>
+    <row r="28" spans="1:13" ht="50.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="121" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="52"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="53"/>
-      <c r="L24" s="65"/>
-    </row>
-    <row r="25" spans="1:13" ht="50.4" x14ac:dyDescent="0.25">
-      <c r="A25" s="64"/>
-      <c r="B25" s="66"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="64"/>
-      <c r="G25" s="48" t="s">
-        <v>60</v>
-      </c>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="66"/>
-      <c r="L25" s="54"/>
-    </row>
-    <row r="26" spans="1:13" ht="63.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="72"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58" t="s">
+      <c r="C28" s="65" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="107"/>
+      <c r="F28" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" s="107"/>
+      <c r="H28" s="107"/>
+      <c r="I28" s="107"/>
+      <c r="J28" s="107"/>
+      <c r="M28" s="102"/>
+    </row>
+    <row r="29" spans="1:13" ht="40.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="98"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="98"/>
+      <c r="D29" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="72"/>
-      <c r="I26" s="72"/>
-      <c r="J26" s="73"/>
-      <c r="L26" s="54"/>
-    </row>
-    <row r="27" spans="1:13" ht="50.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="71" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="70" t="s">
+      <c r="E29" s="98"/>
+      <c r="F29" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="G29" s="98"/>
+      <c r="H29" s="98"/>
+      <c r="I29" s="98"/>
+      <c r="J29" s="98"/>
+      <c r="L29" s="102"/>
+    </row>
+    <row r="30" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="98"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="98"/>
+      <c r="D30" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="80" t="s">
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="98"/>
+      <c r="H30" s="98"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="98"/>
+      <c r="L30" s="102"/>
+    </row>
+    <row r="31" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="98"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="98"/>
+      <c r="D31" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="98"/>
+      <c r="J31" s="98"/>
+      <c r="M31" s="102"/>
+    </row>
+    <row r="32" spans="1:13" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="103"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="103"/>
+      <c r="F32" s="64" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="103"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="103"/>
+      <c r="L32" s="102"/>
+    </row>
+    <row r="33" spans="1:12" ht="45.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="121" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="121" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="68" t="s">
+        <v>95</v>
+      </c>
+      <c r="E33" s="107"/>
+      <c r="F33" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="107"/>
+      <c r="H33" s="107"/>
+      <c r="I33" s="107"/>
+      <c r="J33" s="107"/>
+      <c r="L33" s="108"/>
+    </row>
+    <row r="34" spans="1:12" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="98"/>
+      <c r="B34" s="98"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="80" t="s">
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="98"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="98"/>
+    </row>
+    <row r="35" spans="1:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="103"/>
+      <c r="B35" s="103"/>
+      <c r="C35" s="103"/>
+      <c r="D35" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="103"/>
+      <c r="F35" s="64" t="s">
+        <v>77</v>
+      </c>
+      <c r="G35" s="103"/>
+      <c r="H35" s="103"/>
+      <c r="I35" s="103"/>
+      <c r="J35" s="103"/>
+    </row>
+    <row r="36" spans="1:12" ht="43.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="121" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="121" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="65" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" s="107"/>
+      <c r="F36" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="G36" s="107"/>
+      <c r="H36" s="107"/>
+      <c r="I36" s="107"/>
+      <c r="J36" s="107"/>
+    </row>
+    <row r="37" spans="1:12" ht="35.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="98"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="98"/>
+      <c r="D37" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="98"/>
+      <c r="F37" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="98"/>
+      <c r="H37" s="98"/>
+      <c r="I37" s="98"/>
+      <c r="J37" s="98"/>
+    </row>
+    <row r="38" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="98"/>
+      <c r="B38" s="98"/>
+      <c r="C38" s="98"/>
+      <c r="D38" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="98"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="98"/>
+      <c r="H38" s="98"/>
+      <c r="I38" s="98"/>
+      <c r="J38" s="98"/>
+    </row>
+    <row r="39" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="98"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="98"/>
+      <c r="D39" s="63" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="98"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
+    </row>
+    <row r="40" spans="1:12" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="103"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="103"/>
+      <c r="D40" s="64" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="103"/>
+      <c r="F40" s="64" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="103"/>
+      <c r="H40" s="103"/>
+      <c r="I40" s="103"/>
+      <c r="J40" s="103"/>
+    </row>
+    <row r="41" spans="1:12" ht="41.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="121" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="121" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="107"/>
+      <c r="F41" s="65" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" s="107"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="107"/>
+      <c r="J41" s="107"/>
+    </row>
+    <row r="42" spans="1:12" ht="27" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="98"/>
+      <c r="B42" s="98"/>
+      <c r="C42" s="98"/>
+      <c r="D42" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="E42" s="98"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="98"/>
+      <c r="H42" s="98"/>
+      <c r="I42" s="98"/>
+      <c r="J42" s="98"/>
+    </row>
+    <row r="43" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="103"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="103"/>
+      <c r="D43" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="103"/>
+      <c r="F43" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="G43" s="103"/>
+      <c r="H43" s="103"/>
+      <c r="I43" s="103"/>
+      <c r="J43" s="103"/>
+    </row>
+    <row r="44" spans="1:12" ht="41.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="121" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="121" t="s">
         <v>97</v>
       </c>
-      <c r="E27" s="70"/>
-      <c r="F27" s="76" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="70"/>
-      <c r="M27" s="62"/>
-    </row>
-    <row r="28" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="64"/>
-      <c r="B28" s="64"/>
-      <c r="C28" s="64"/>
-      <c r="D28" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="64"/>
-      <c r="F28" s="77" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="64"/>
-      <c r="J28" s="64"/>
-      <c r="L28" s="54"/>
-    </row>
-    <row r="29" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="64"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="69" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="64"/>
-      <c r="J29" s="64"/>
-      <c r="L29" s="54"/>
-    </row>
-    <row r="30" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="64"/>
-      <c r="B30" s="64"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="69" t="s">
-        <v>69</v>
-      </c>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="64"/>
-      <c r="J30" s="64"/>
-      <c r="M30" s="62" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="72"/>
-      <c r="B31" s="72"/>
-      <c r="C31" s="72"/>
-      <c r="D31" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="E31" s="72"/>
-      <c r="F31" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="G31" s="72"/>
-      <c r="H31" s="72"/>
-      <c r="I31" s="72"/>
-      <c r="J31" s="72"/>
-      <c r="L31" s="54" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="45.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="71" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="71" t="s">
-        <v>75</v>
-      </c>
-      <c r="C32" s="80" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="83" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="70"/>
-      <c r="F32" s="80" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="70"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="70"/>
-      <c r="L32" s="45" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="64"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="81" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-    </row>
-    <row r="34" spans="1:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="72"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="82" t="s">
-        <v>80</v>
-      </c>
-      <c r="E34" s="72"/>
-      <c r="F34" s="79" t="s">
-        <v>79</v>
-      </c>
-      <c r="G34" s="72"/>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="72"/>
-    </row>
-    <row r="35" spans="1:10" ht="43.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="71" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="71" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="80" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="80" t="s">
-        <v>97</v>
-      </c>
-      <c r="E35" s="70"/>
-      <c r="F35" s="80" t="s">
-        <v>71</v>
-      </c>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-    </row>
-    <row r="36" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="64"/>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="69" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" s="64"/>
-      <c r="F36" s="77" t="s">
-        <v>72</v>
-      </c>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-      <c r="I36" s="64"/>
-      <c r="J36" s="64"/>
-    </row>
-    <row r="37" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="64"/>
-      <c r="B37" s="64"/>
-      <c r="C37" s="64"/>
-      <c r="D37" s="69" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="64"/>
-      <c r="I37" s="64"/>
-      <c r="J37" s="64"/>
-    </row>
-    <row r="38" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="64"/>
-      <c r="B38" s="64"/>
-      <c r="C38" s="64"/>
-      <c r="D38" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" s="64"/>
-      <c r="F38" s="64"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="64"/>
-      <c r="J38" s="64"/>
-    </row>
-    <row r="39" spans="1:10" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="72"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="E39" s="72"/>
-      <c r="F39" s="79" t="s">
-        <v>88</v>
-      </c>
-      <c r="G39" s="72"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-    </row>
-    <row r="40" spans="1:10" ht="40.200000000000003" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="71" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" s="71" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="80" t="s">
-        <v>91</v>
-      </c>
-      <c r="D40" s="80" t="s">
-        <v>92</v>
-      </c>
-      <c r="E40" s="70"/>
-      <c r="F40" s="80" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="70"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="70"/>
-      <c r="J40" s="70"/>
-    </row>
-    <row r="41" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A41" s="64"/>
-      <c r="B41" s="64"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="77" t="s">
-        <v>93</v>
-      </c>
-      <c r="E41" s="64"/>
-      <c r="F41" s="64"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="64"/>
-      <c r="I41" s="64"/>
-      <c r="J41" s="64"/>
-    </row>
-    <row r="42" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="72"/>
-      <c r="B42" s="72"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="79" t="s">
+      <c r="C44" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="65" t="s">
+        <v>99</v>
+      </c>
+      <c r="E44" s="107"/>
+      <c r="F44" s="65" t="s">
+        <v>100</v>
+      </c>
+      <c r="G44" s="107"/>
+      <c r="H44" s="107"/>
+      <c r="I44" s="107"/>
+      <c r="J44" s="107"/>
+    </row>
+    <row r="45" spans="1:12" ht="53.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="98"/>
+      <c r="B45" s="98"/>
+      <c r="C45" s="98"/>
+      <c r="D45" s="63" t="s">
+        <v>101</v>
+      </c>
+      <c r="E45" s="98" t="s">
+        <v>103</v>
+      </c>
+      <c r="F45" s="98" t="s">
+        <v>104</v>
+      </c>
+      <c r="G45" s="98"/>
+      <c r="H45" s="98"/>
+      <c r="I45" s="98"/>
+      <c r="J45" s="98"/>
+    </row>
+    <row r="46" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="103"/>
+      <c r="B46" s="103"/>
+      <c r="C46" s="103"/>
+      <c r="D46" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="103"/>
+      <c r="F46" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="E42" s="72"/>
-      <c r="F42" s="79" t="s">
-        <v>96</v>
-      </c>
-      <c r="G42" s="72"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-    </row>
-    <row r="43" spans="1:10" ht="40.200000000000003" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="71" t="s">
-        <v>98</v>
-      </c>
-      <c r="B43" s="71" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="80" t="s">
-        <v>91</v>
-      </c>
-      <c r="D43" s="80" t="s">
-        <v>92</v>
-      </c>
-      <c r="E43" s="70"/>
-      <c r="F43" s="80" t="s">
-        <v>95</v>
-      </c>
-      <c r="G43" s="70"/>
-      <c r="H43" s="70"/>
-      <c r="I43" s="70"/>
-      <c r="J43" s="70"/>
-    </row>
-    <row r="44" spans="1:10" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A44" s="64"/>
-      <c r="B44" s="64"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="77" t="s">
-        <v>93</v>
-      </c>
-      <c r="E44" s="64"/>
-      <c r="F44" s="64"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="64"/>
-      <c r="I44" s="64"/>
-      <c r="J44" s="64"/>
-    </row>
-    <row r="45" spans="1:10" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="72"/>
-      <c r="B45" s="72"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="79" t="s">
-        <v>94</v>
-      </c>
-      <c r="E45" s="72"/>
-      <c r="F45" s="79" t="s">
-        <v>96</v>
-      </c>
-      <c r="G45" s="72"/>
-      <c r="H45" s="72"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="72"/>
-    </row>
-    <row r="46" spans="1:10" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="G46" s="103"/>
+      <c r="H46" s="103"/>
+      <c r="I46" s="103"/>
+      <c r="J46" s="103"/>
+    </row>
+    <row r="47" spans="1:12" ht="13.8" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="G17:G20"/>
+    <mergeCell ref="G18:G21"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B6:I6"/>
     <mergeCell ref="B7:I7"/>
     <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="G15:G17"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>